<commit_message>
updated fakeout to match mql5 code
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Desktop/Fulfillment/Forex - Algo trading/Python API/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F524EEA8-73B1-B649-B451-CEC7E200240E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59913B24-2E98-1C42-932B-43BEF1B4EF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18580" yWindow="29840" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
   <si>
     <t>strategy_name</t>
   </si>
@@ -588,9 +588,6 @@
   </si>
   <si>
     <t>optimize</t>
-  </si>
-  <si>
-    <t>EURUSD</t>
   </si>
   <si>
     <t>Indicator</t>
@@ -660,7 +657,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -782,6 +779,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Intel Clear"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1150,7 +1153,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1170,6 +1173,7 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1533,50 +1537,50 @@
   <dimension ref="A1:CT386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="BD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CS3" sqref="CS3"/>
+      <selection pane="bottomRight" activeCell="CT3" sqref="CT3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="6" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="13.5" customWidth="1"/>
-    <col min="12" max="12" width="6.5" customWidth="1"/>
-    <col min="13" max="13" width="7.1640625" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" customWidth="1"/>
-    <col min="15" max="15" width="8.1640625" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" customWidth="1"/>
-    <col min="19" max="22" width="9.1640625" customWidth="1"/>
-    <col min="53" max="53" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16.6640625" customWidth="1"/>
-    <col min="67" max="67" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" customWidth="1"/>
+    <col min="19" max="22" width="9.140625" customWidth="1"/>
+    <col min="53" max="53" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.7109375" customWidth="1"/>
+    <col min="67" max="67" width="9.42578125" customWidth="1"/>
     <col min="69" max="69" width="10" customWidth="1"/>
-    <col min="70" max="70" width="9.5" customWidth="1"/>
-    <col min="80" max="80" width="10.33203125" customWidth="1"/>
-    <col min="82" max="82" width="11.5" customWidth="1"/>
-    <col min="83" max="83" width="10.5" customWidth="1"/>
+    <col min="70" max="70" width="9.42578125" customWidth="1"/>
+    <col min="80" max="80" width="10.28515625" customWidth="1"/>
+    <col min="82" max="82" width="11.42578125" customWidth="1"/>
+    <col min="83" max="83" width="10.42578125" customWidth="1"/>
     <col min="84" max="85" width="11" customWidth="1"/>
-    <col min="86" max="86" width="10.5" customWidth="1"/>
-    <col min="87" max="87" width="10.1640625" customWidth="1"/>
-    <col min="88" max="88" width="11.83203125" customWidth="1"/>
-    <col min="89" max="89" width="11.5" customWidth="1"/>
-    <col min="90" max="90" width="10.83203125" customWidth="1"/>
-    <col min="91" max="91" width="10.6640625" customWidth="1"/>
-    <col min="92" max="92" width="12.83203125" customWidth="1"/>
-    <col min="93" max="93" width="13.5" customWidth="1"/>
-    <col min="95" max="95" width="9.6640625" customWidth="1"/>
-    <col min="97" max="97" width="10.6640625" customWidth="1"/>
+    <col min="86" max="86" width="10.42578125" customWidth="1"/>
+    <col min="87" max="87" width="10.140625" customWidth="1"/>
+    <col min="88" max="88" width="11.85546875" customWidth="1"/>
+    <col min="89" max="89" width="11.42578125" customWidth="1"/>
+    <col min="90" max="90" width="10.85546875" customWidth="1"/>
+    <col min="91" max="91" width="10.7109375" customWidth="1"/>
+    <col min="92" max="92" width="12.85546875" customWidth="1"/>
+    <col min="93" max="93" width="13.42578125" customWidth="1"/>
+    <col min="95" max="95" width="9.7109375" customWidth="1"/>
+    <col min="97" max="97" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:98" s="1" customFormat="1" ht="63" customHeight="1">
@@ -1599,7 +1603,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1800,7 +1804,7 @@
         <v>135</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BW1" s="1" t="s">
         <v>66</v>
@@ -1886,7 +1890,7 @@
         <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1895,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1910,10 +1914,10 @@
         <v>110</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N2" t="s">
         <v>128</v>
@@ -1925,7 +1929,7 @@
         <v>196</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T2" s="8">
         <v>1</v>
@@ -1937,7 +1941,7 @@
         <v>0.25</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Y2" s="8" t="s">
         <v>132</v>
@@ -1985,16 +1989,16 @@
         <v>0.5</v>
       </c>
       <c r="BN2" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="BO2">
         <v>0</v>
       </c>
       <c r="BP2" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="BR2" s="8">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="BS2">
         <v>5000</v>
@@ -2006,7 +2010,7 @@
         <v>20</v>
       </c>
       <c r="BV2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="BW2" t="s">
         <v>67</v>
@@ -2018,10 +2022,10 @@
         <v>14</v>
       </c>
       <c r="CQ2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="CR2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="CS2" s="5">
         <v>45292</v>
@@ -2035,7 +2039,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -2044,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2055,15 +2065,128 @@
       <c r="J3">
         <v>24</v>
       </c>
-      <c r="CS3" s="5"/>
+      <c r="K3" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M3" t="s">
+        <v>195</v>
+      </c>
+      <c r="N3" t="s">
+        <v>128</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="R3" t="s">
+        <v>196</v>
+      </c>
+      <c r="S3" t="s">
+        <v>195</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>195</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC3">
+        <v>100</v>
+      </c>
+      <c r="AD3">
+        <v>3</v>
+      </c>
+      <c r="AE3">
+        <v>10</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>2</v>
+      </c>
+      <c r="AH3">
+        <v>3</v>
+      </c>
+      <c r="AI3">
+        <v>200</v>
+      </c>
+      <c r="AJ3">
+        <v>0.1</v>
+      </c>
+      <c r="AK3" s="11">
+        <v>2</v>
+      </c>
+      <c r="AL3">
+        <v>2</v>
+      </c>
+      <c r="AM3">
+        <v>0.5</v>
+      </c>
+      <c r="BN3" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="BO3">
+        <v>0</v>
+      </c>
+      <c r="BP3" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="BR3">
+        <v>25</v>
+      </c>
+      <c r="BS3">
+        <v>5000</v>
+      </c>
+      <c r="BT3">
+        <v>20</v>
+      </c>
+      <c r="BU3">
+        <v>20</v>
+      </c>
+      <c r="CP3">
+        <v>14</v>
+      </c>
+      <c r="CQ3">
+        <v>45</v>
+      </c>
+      <c r="CR3">
+        <v>45</v>
+      </c>
+      <c r="CS3" s="5">
+        <v>43831</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:98">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>127</v>
-      </c>
       <c r="CS4" s="5"/>
     </row>
     <row r="5" spans="1:98">
@@ -2172,6 +2295,9 @@
       <c r="CS22" s="5"/>
     </row>
     <row r="23" spans="1:97">
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
       <c r="CS23" s="5"/>
     </row>
     <row r="24" spans="1:97">
@@ -3291,7 +3417,7 @@
           <x14:formula1>
             <xm:f>validation!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>CP51:CP1048576 L2:M1048576 BP2:BP1048576 R2:R266 S2:S380 W2:W385 BN2:BN385 G2:G374</xm:sqref>
+          <xm:sqref>CP51:CP1048576 L2:M1048576 BN2:BN385 R2:R266 S2:S380 W2:W385 G2:G374 BP2:BP1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
@@ -3392,10 +3518,10 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="8" max="9" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="8" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="34">
@@ -3443,7 +3569,7 @@
         <v>98</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -3478,7 +3604,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -3749,18 +3875,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -3768,7 +3894,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -3776,29 +3902,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3818,24 +3944,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
         <v>198</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>199</v>
-      </c>
-      <c r="C1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
         <v>201</v>
-      </c>
-      <c r="C2" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split all range strategies to buy and sell methods - fixed fakuout only takes buy trades
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850627D1-99F3-FA4C-B042-7892EB9B2A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B9CF64-749F-4440-AD22-7E0B9FFF092E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="206">
   <si>
     <t>strategy_name</t>
   </si>
@@ -647,10 +647,13 @@
     <t>exitP_daily_candle_exit_hour</t>
   </si>
   <si>
-    <t>FakeOut_D</t>
-  </si>
-  <si>
     <t>tradeP_fixed_order_size</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>FakeOut_H</t>
   </si>
 </sst>
 </file>
@@ -1537,10 +1540,10 @@
   <dimension ref="A1:CT386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CP2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="CR2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CS5" sqref="CS5"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -1603,7 +1606,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1887,7 +1890,7 @@
         <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
         <v>127</v>
@@ -1896,7 +1899,7 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G2" t="s">
         <v>195</v>
@@ -2031,7 +2034,7 @@
         <v>43831</v>
       </c>
       <c r="CT2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:98">
@@ -2039,19 +2042,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
         <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>204</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G3" t="s">
         <v>195</v>
@@ -2180,7 +2183,7 @@
         <v>43831</v>
       </c>
       <c r="CT3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:98">

</xml_diff>

<commit_message>
updated profit to account for base currency in backtesting
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934FB410-B596-244F-9EA5-A0B6347D88C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D82A1F9-B375-594B-8644-B00D0E1D1669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,7 +788,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -976,18 +976,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF40FF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1153,7 +1141,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1162,18 +1150,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1540,7 +1529,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -1583,349 +1572,349 @@
     <col min="97" max="97" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="1" customFormat="1" ht="63" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:98" s="7" customFormat="1" ht="63" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="7" t="s">
         <v>26</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AY1" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="AZ1" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BA1" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BB1" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BC1" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BD1" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BE1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BF1" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BG1" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BH1" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BI1" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BK1" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BL1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BM1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BN1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BO1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BP1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BQ1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BR1" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BS1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BT1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BU1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BV1" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BW1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BX1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BY1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="BZ1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CA1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CB1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CC1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CD1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CE1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CF1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CG1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CH1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CI1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CJ1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CK1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CL1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CM1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CN1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CO1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CP1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CQ1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CR1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CS1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CT1" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
-      <c r="A2">
+    <row r="2" spans="1:98" s="8" customFormat="1">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>182</v>
       </c>
       <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>0.1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="8">
         <v>2</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="8">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="8">
         <v>10</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="10" t="s">
         <v>196</v>
       </c>
       <c r="S2" s="10" t="s">
@@ -1940,13 +1929,13 @@
       <c r="V2" s="8">
         <v>0.25</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="10" t="s">
         <v>196</v>
       </c>
       <c r="Y2" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="8">
         <v>2</v>
       </c>
       <c r="AA2" s="8" t="s">
@@ -1988,50 +1977,50 @@
       <c r="AM2" s="8">
         <v>0.5</v>
       </c>
-      <c r="BN2" s="9" t="s">
+      <c r="BN2" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="BO2">
+      <c r="BO2" s="8">
         <v>0</v>
       </c>
-      <c r="BP2" s="9" t="s">
+      <c r="BP2" s="10" t="s">
         <v>196</v>
       </c>
       <c r="BR2" s="8">
         <v>25</v>
       </c>
-      <c r="BS2">
+      <c r="BS2" s="8">
         <v>5000</v>
       </c>
-      <c r="BT2">
+      <c r="BT2" s="8">
         <v>20</v>
       </c>
-      <c r="BU2">
+      <c r="BU2" s="8">
         <v>20</v>
       </c>
-      <c r="BV2">
+      <c r="BV2" s="8">
         <v>22</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BW2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="BX2">
+      <c r="BX2" s="8">
         <v>1</v>
       </c>
-      <c r="CP2">
+      <c r="CP2" s="8">
         <v>14</v>
       </c>
-      <c r="CQ2">
+      <c r="CQ2" s="8">
         <v>45</v>
       </c>
-      <c r="CR2">
+      <c r="CR2" s="8">
         <v>45</v>
       </c>
-      <c r="CS2" s="5">
+      <c r="CS2" s="11">
         <v>43831</v>
       </c>
-      <c r="CT2" t="s">
-        <v>7</v>
+      <c r="CT2" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:98">
@@ -2042,7 +2031,7 @@
         <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
         <v>127</v>
@@ -2137,7 +2126,7 @@
       <c r="AJ3">
         <v>0.1</v>
       </c>
-      <c r="AK3" s="11">
+      <c r="AK3" s="6">
         <v>2</v>
       </c>
       <c r="AL3">
@@ -2146,13 +2135,13 @@
       <c r="AM3">
         <v>0.5</v>
       </c>
-      <c r="BN3" s="9" t="s">
+      <c r="BN3" s="5" t="s">
         <v>196</v>
       </c>
       <c r="BO3">
         <v>0</v>
       </c>
-      <c r="BP3" s="9" t="s">
+      <c r="BP3" s="5" t="s">
         <v>196</v>
       </c>
       <c r="BR3">
@@ -2176,7 +2165,7 @@
       <c r="CR3">
         <v>45</v>
       </c>
-      <c r="CS3" s="5">
+      <c r="CS3" s="4">
         <v>43831</v>
       </c>
       <c r="CT3" t="s">
@@ -2187,1207 +2176,1207 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="CS4" s="5"/>
+      <c r="CS4" s="4"/>
     </row>
     <row r="5" spans="1:98">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="CS5" s="5"/>
+      <c r="CS5" s="4"/>
     </row>
     <row r="6" spans="1:98">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="CS6" s="5"/>
+      <c r="CS6" s="4"/>
     </row>
     <row r="7" spans="1:98">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="CS7" s="5"/>
+      <c r="CS7" s="4"/>
     </row>
     <row r="8" spans="1:98">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="CS8" s="5"/>
+      <c r="CS8" s="4"/>
     </row>
     <row r="9" spans="1:98">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="CS9" s="5"/>
+      <c r="CS9" s="4"/>
     </row>
     <row r="10" spans="1:98">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="CS10" s="5"/>
+      <c r="CS10" s="4"/>
     </row>
     <row r="11" spans="1:98">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="CS11" s="5"/>
+      <c r="CS11" s="4"/>
     </row>
     <row r="12" spans="1:98">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="CS12" s="5"/>
+      <c r="CS12" s="4"/>
     </row>
     <row r="13" spans="1:98">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="CS13" s="5"/>
+      <c r="CS13" s="4"/>
     </row>
     <row r="14" spans="1:98">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="CS14" s="5"/>
+      <c r="CS14" s="4"/>
     </row>
     <row r="15" spans="1:98">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="CS15" s="5"/>
+      <c r="CS15" s="4"/>
     </row>
     <row r="16" spans="1:98">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="CS16" s="5"/>
+      <c r="CS16" s="4"/>
     </row>
     <row r="17" spans="1:97">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="CS17" s="5"/>
+      <c r="CS17" s="4"/>
     </row>
     <row r="18" spans="1:97">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="CS18" s="5"/>
+      <c r="CS18" s="4"/>
     </row>
     <row r="19" spans="1:97">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="CS19" s="5"/>
+      <c r="CS19" s="4"/>
     </row>
     <row r="20" spans="1:97">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="CS20" s="5"/>
+      <c r="CS20" s="4"/>
     </row>
     <row r="21" spans="1:97">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="CS21" s="5"/>
+      <c r="CS21" s="4"/>
     </row>
     <row r="22" spans="1:97">
-      <c r="CS22" s="5"/>
+      <c r="CS22" s="4"/>
     </row>
     <row r="23" spans="1:97">
       <c r="D23" t="s">
         <v>127</v>
       </c>
-      <c r="CS23" s="5"/>
+      <c r="CS23" s="4"/>
     </row>
     <row r="24" spans="1:97">
-      <c r="CS24" s="5"/>
+      <c r="CS24" s="4"/>
     </row>
     <row r="25" spans="1:97">
-      <c r="CS25" s="5"/>
+      <c r="CS25" s="4"/>
     </row>
     <row r="26" spans="1:97">
-      <c r="CS26" s="5"/>
+      <c r="CS26" s="4"/>
     </row>
     <row r="27" spans="1:97">
-      <c r="CS27" s="5"/>
+      <c r="CS27" s="4"/>
     </row>
     <row r="28" spans="1:97">
-      <c r="CS28" s="5"/>
+      <c r="CS28" s="4"/>
     </row>
     <row r="29" spans="1:97">
-      <c r="CS29" s="5"/>
+      <c r="CS29" s="4"/>
     </row>
     <row r="30" spans="1:97">
-      <c r="CS30" s="5"/>
+      <c r="CS30" s="4"/>
     </row>
     <row r="31" spans="1:97">
-      <c r="CS31" s="5"/>
+      <c r="CS31" s="4"/>
     </row>
     <row r="32" spans="1:97">
-      <c r="CS32" s="5"/>
+      <c r="CS32" s="4"/>
     </row>
     <row r="33" spans="97:97">
-      <c r="CS33" s="5"/>
+      <c r="CS33" s="4"/>
     </row>
     <row r="34" spans="97:97">
-      <c r="CS34" s="5"/>
+      <c r="CS34" s="4"/>
     </row>
     <row r="35" spans="97:97">
-      <c r="CS35" s="5"/>
+      <c r="CS35" s="4"/>
     </row>
     <row r="36" spans="97:97">
-      <c r="CS36" s="5"/>
+      <c r="CS36" s="4"/>
     </row>
     <row r="37" spans="97:97">
-      <c r="CS37" s="5"/>
+      <c r="CS37" s="4"/>
     </row>
     <row r="38" spans="97:97">
-      <c r="CS38" s="5"/>
+      <c r="CS38" s="4"/>
     </row>
     <row r="39" spans="97:97">
-      <c r="CS39" s="5"/>
+      <c r="CS39" s="4"/>
     </row>
     <row r="40" spans="97:97">
-      <c r="CS40" s="5"/>
+      <c r="CS40" s="4"/>
     </row>
     <row r="41" spans="97:97">
-      <c r="CS41" s="5"/>
+      <c r="CS41" s="4"/>
     </row>
     <row r="42" spans="97:97">
-      <c r="CS42" s="5"/>
+      <c r="CS42" s="4"/>
     </row>
     <row r="43" spans="97:97">
-      <c r="CS43" s="5"/>
+      <c r="CS43" s="4"/>
     </row>
     <row r="44" spans="97:97">
-      <c r="CS44" s="5"/>
+      <c r="CS44" s="4"/>
     </row>
     <row r="45" spans="97:97">
-      <c r="CS45" s="5"/>
+      <c r="CS45" s="4"/>
     </row>
     <row r="46" spans="97:97">
-      <c r="CS46" s="5"/>
+      <c r="CS46" s="4"/>
     </row>
     <row r="47" spans="97:97">
-      <c r="CS47" s="5"/>
+      <c r="CS47" s="4"/>
     </row>
     <row r="48" spans="97:97">
-      <c r="CS48" s="5"/>
+      <c r="CS48" s="4"/>
     </row>
     <row r="49" spans="97:97">
-      <c r="CS49" s="5"/>
+      <c r="CS49" s="4"/>
     </row>
     <row r="50" spans="97:97">
-      <c r="CS50" s="5"/>
+      <c r="CS50" s="4"/>
     </row>
     <row r="51" spans="97:97">
-      <c r="CS51" s="5"/>
+      <c r="CS51" s="4"/>
     </row>
     <row r="52" spans="97:97">
-      <c r="CS52" s="5"/>
+      <c r="CS52" s="4"/>
     </row>
     <row r="53" spans="97:97">
-      <c r="CS53" s="5"/>
+      <c r="CS53" s="4"/>
     </row>
     <row r="54" spans="97:97">
-      <c r="CS54" s="5"/>
+      <c r="CS54" s="4"/>
     </row>
     <row r="55" spans="97:97">
-      <c r="CS55" s="5"/>
+      <c r="CS55" s="4"/>
     </row>
     <row r="56" spans="97:97">
-      <c r="CS56" s="5"/>
+      <c r="CS56" s="4"/>
     </row>
     <row r="57" spans="97:97">
-      <c r="CS57" s="5"/>
+      <c r="CS57" s="4"/>
     </row>
     <row r="58" spans="97:97">
-      <c r="CS58" s="5"/>
+      <c r="CS58" s="4"/>
     </row>
     <row r="59" spans="97:97">
-      <c r="CS59" s="5"/>
+      <c r="CS59" s="4"/>
     </row>
     <row r="60" spans="97:97">
-      <c r="CS60" s="5"/>
+      <c r="CS60" s="4"/>
     </row>
     <row r="61" spans="97:97">
-      <c r="CS61" s="5"/>
+      <c r="CS61" s="4"/>
     </row>
     <row r="62" spans="97:97">
-      <c r="CS62" s="5"/>
+      <c r="CS62" s="4"/>
     </row>
     <row r="63" spans="97:97">
-      <c r="CS63" s="5"/>
+      <c r="CS63" s="4"/>
     </row>
     <row r="64" spans="97:97">
-      <c r="CS64" s="5"/>
+      <c r="CS64" s="4"/>
     </row>
     <row r="65" spans="97:97">
-      <c r="CS65" s="5"/>
+      <c r="CS65" s="4"/>
     </row>
     <row r="66" spans="97:97">
-      <c r="CS66" s="5"/>
+      <c r="CS66" s="4"/>
     </row>
     <row r="67" spans="97:97">
-      <c r="CS67" s="5"/>
+      <c r="CS67" s="4"/>
     </row>
     <row r="68" spans="97:97">
-      <c r="CS68" s="5"/>
+      <c r="CS68" s="4"/>
     </row>
     <row r="69" spans="97:97">
-      <c r="CS69" s="5"/>
+      <c r="CS69" s="4"/>
     </row>
     <row r="70" spans="97:97">
-      <c r="CS70" s="5"/>
+      <c r="CS70" s="4"/>
     </row>
     <row r="71" spans="97:97">
-      <c r="CS71" s="5"/>
+      <c r="CS71" s="4"/>
     </row>
     <row r="72" spans="97:97">
-      <c r="CS72" s="5"/>
+      <c r="CS72" s="4"/>
     </row>
     <row r="73" spans="97:97">
-      <c r="CS73" s="5"/>
+      <c r="CS73" s="4"/>
     </row>
     <row r="74" spans="97:97">
-      <c r="CS74" s="5"/>
+      <c r="CS74" s="4"/>
     </row>
     <row r="75" spans="97:97">
-      <c r="CS75" s="5"/>
+      <c r="CS75" s="4"/>
     </row>
     <row r="76" spans="97:97">
-      <c r="CS76" s="5"/>
+      <c r="CS76" s="4"/>
     </row>
     <row r="77" spans="97:97">
-      <c r="CS77" s="5"/>
+      <c r="CS77" s="4"/>
     </row>
     <row r="78" spans="97:97">
-      <c r="CS78" s="5"/>
+      <c r="CS78" s="4"/>
     </row>
     <row r="79" spans="97:97">
-      <c r="CS79" s="5"/>
+      <c r="CS79" s="4"/>
     </row>
     <row r="80" spans="97:97">
-      <c r="CS80" s="5"/>
+      <c r="CS80" s="4"/>
     </row>
     <row r="81" spans="97:97">
-      <c r="CS81" s="5"/>
+      <c r="CS81" s="4"/>
     </row>
     <row r="82" spans="97:97">
-      <c r="CS82" s="5"/>
+      <c r="CS82" s="4"/>
     </row>
     <row r="83" spans="97:97">
-      <c r="CS83" s="5"/>
+      <c r="CS83" s="4"/>
     </row>
     <row r="84" spans="97:97">
-      <c r="CS84" s="5"/>
+      <c r="CS84" s="4"/>
     </row>
     <row r="85" spans="97:97">
-      <c r="CS85" s="5"/>
+      <c r="CS85" s="4"/>
     </row>
     <row r="86" spans="97:97">
-      <c r="CS86" s="5"/>
+      <c r="CS86" s="4"/>
     </row>
     <row r="87" spans="97:97">
-      <c r="CS87" s="5"/>
+      <c r="CS87" s="4"/>
     </row>
     <row r="88" spans="97:97">
-      <c r="CS88" s="5"/>
+      <c r="CS88" s="4"/>
     </row>
     <row r="89" spans="97:97">
-      <c r="CS89" s="5"/>
+      <c r="CS89" s="4"/>
     </row>
     <row r="90" spans="97:97">
-      <c r="CS90" s="5"/>
+      <c r="CS90" s="4"/>
     </row>
     <row r="91" spans="97:97">
-      <c r="CS91" s="5"/>
+      <c r="CS91" s="4"/>
     </row>
     <row r="92" spans="97:97">
-      <c r="CS92" s="5"/>
+      <c r="CS92" s="4"/>
     </row>
     <row r="93" spans="97:97">
-      <c r="CS93" s="5"/>
+      <c r="CS93" s="4"/>
     </row>
     <row r="94" spans="97:97">
-      <c r="CS94" s="5"/>
+      <c r="CS94" s="4"/>
     </row>
     <row r="95" spans="97:97">
-      <c r="CS95" s="5"/>
+      <c r="CS95" s="4"/>
     </row>
     <row r="96" spans="97:97">
-      <c r="CS96" s="5"/>
+      <c r="CS96" s="4"/>
     </row>
     <row r="97" spans="97:97">
-      <c r="CS97" s="5"/>
+      <c r="CS97" s="4"/>
     </row>
     <row r="98" spans="97:97">
-      <c r="CS98" s="5"/>
+      <c r="CS98" s="4"/>
     </row>
     <row r="99" spans="97:97">
-      <c r="CS99" s="5"/>
+      <c r="CS99" s="4"/>
     </row>
     <row r="100" spans="97:97">
-      <c r="CS100" s="5"/>
+      <c r="CS100" s="4"/>
     </row>
     <row r="101" spans="97:97">
-      <c r="CS101" s="5"/>
+      <c r="CS101" s="4"/>
     </row>
     <row r="102" spans="97:97">
-      <c r="CS102" s="5"/>
+      <c r="CS102" s="4"/>
     </row>
     <row r="103" spans="97:97">
-      <c r="CS103" s="5"/>
+      <c r="CS103" s="4"/>
     </row>
     <row r="104" spans="97:97">
-      <c r="CS104" s="5"/>
+      <c r="CS104" s="4"/>
     </row>
     <row r="105" spans="97:97">
-      <c r="CS105" s="5"/>
+      <c r="CS105" s="4"/>
     </row>
     <row r="106" spans="97:97">
-      <c r="CS106" s="5"/>
+      <c r="CS106" s="4"/>
     </row>
     <row r="107" spans="97:97">
-      <c r="CS107" s="5"/>
+      <c r="CS107" s="4"/>
     </row>
     <row r="108" spans="97:97">
-      <c r="CS108" s="5"/>
+      <c r="CS108" s="4"/>
     </row>
     <row r="109" spans="97:97">
-      <c r="CS109" s="5"/>
+      <c r="CS109" s="4"/>
     </row>
     <row r="110" spans="97:97">
-      <c r="CS110" s="5"/>
+      <c r="CS110" s="4"/>
     </row>
     <row r="111" spans="97:97">
-      <c r="CS111" s="5"/>
+      <c r="CS111" s="4"/>
     </row>
     <row r="112" spans="97:97">
-      <c r="CS112" s="5"/>
+      <c r="CS112" s="4"/>
     </row>
     <row r="113" spans="97:97">
-      <c r="CS113" s="5"/>
+      <c r="CS113" s="4"/>
     </row>
     <row r="114" spans="97:97">
-      <c r="CS114" s="5"/>
+      <c r="CS114" s="4"/>
     </row>
     <row r="115" spans="97:97">
-      <c r="CS115" s="5"/>
+      <c r="CS115" s="4"/>
     </row>
     <row r="116" spans="97:97">
-      <c r="CS116" s="5"/>
+      <c r="CS116" s="4"/>
     </row>
     <row r="117" spans="97:97">
-      <c r="CS117" s="5"/>
+      <c r="CS117" s="4"/>
     </row>
     <row r="118" spans="97:97">
-      <c r="CS118" s="5"/>
+      <c r="CS118" s="4"/>
     </row>
     <row r="119" spans="97:97">
-      <c r="CS119" s="5"/>
+      <c r="CS119" s="4"/>
     </row>
     <row r="120" spans="97:97">
-      <c r="CS120" s="5"/>
+      <c r="CS120" s="4"/>
     </row>
     <row r="121" spans="97:97">
-      <c r="CS121" s="5"/>
+      <c r="CS121" s="4"/>
     </row>
     <row r="122" spans="97:97">
-      <c r="CS122" s="5"/>
+      <c r="CS122" s="4"/>
     </row>
     <row r="123" spans="97:97">
-      <c r="CS123" s="5"/>
+      <c r="CS123" s="4"/>
     </row>
     <row r="124" spans="97:97">
-      <c r="CS124" s="5"/>
+      <c r="CS124" s="4"/>
     </row>
     <row r="125" spans="97:97">
-      <c r="CS125" s="5"/>
+      <c r="CS125" s="4"/>
     </row>
     <row r="126" spans="97:97">
-      <c r="CS126" s="5"/>
+      <c r="CS126" s="4"/>
     </row>
     <row r="127" spans="97:97">
-      <c r="CS127" s="5"/>
+      <c r="CS127" s="4"/>
     </row>
     <row r="128" spans="97:97">
-      <c r="CS128" s="5"/>
+      <c r="CS128" s="4"/>
     </row>
     <row r="129" spans="97:97">
-      <c r="CS129" s="5"/>
+      <c r="CS129" s="4"/>
     </row>
     <row r="130" spans="97:97">
-      <c r="CS130" s="5"/>
+      <c r="CS130" s="4"/>
     </row>
     <row r="131" spans="97:97">
-      <c r="CS131" s="5"/>
+      <c r="CS131" s="4"/>
     </row>
     <row r="132" spans="97:97">
-      <c r="CS132" s="5"/>
+      <c r="CS132" s="4"/>
     </row>
     <row r="133" spans="97:97">
-      <c r="CS133" s="5"/>
+      <c r="CS133" s="4"/>
     </row>
     <row r="134" spans="97:97">
-      <c r="CS134" s="5"/>
+      <c r="CS134" s="4"/>
     </row>
     <row r="135" spans="97:97">
-      <c r="CS135" s="5"/>
+      <c r="CS135" s="4"/>
     </row>
     <row r="136" spans="97:97">
-      <c r="CS136" s="5"/>
+      <c r="CS136" s="4"/>
     </row>
     <row r="137" spans="97:97">
-      <c r="CS137" s="5"/>
+      <c r="CS137" s="4"/>
     </row>
     <row r="138" spans="97:97">
-      <c r="CS138" s="5"/>
+      <c r="CS138" s="4"/>
     </row>
     <row r="139" spans="97:97">
-      <c r="CS139" s="5"/>
+      <c r="CS139" s="4"/>
     </row>
     <row r="140" spans="97:97">
-      <c r="CS140" s="5"/>
+      <c r="CS140" s="4"/>
     </row>
     <row r="141" spans="97:97">
-      <c r="CS141" s="5"/>
+      <c r="CS141" s="4"/>
     </row>
     <row r="142" spans="97:97">
-      <c r="CS142" s="5"/>
+      <c r="CS142" s="4"/>
     </row>
     <row r="143" spans="97:97">
-      <c r="CS143" s="5"/>
+      <c r="CS143" s="4"/>
     </row>
     <row r="144" spans="97:97">
-      <c r="CS144" s="5"/>
+      <c r="CS144" s="4"/>
     </row>
     <row r="145" spans="97:97">
-      <c r="CS145" s="5"/>
+      <c r="CS145" s="4"/>
     </row>
     <row r="146" spans="97:97">
-      <c r="CS146" s="5"/>
+      <c r="CS146" s="4"/>
     </row>
     <row r="147" spans="97:97">
-      <c r="CS147" s="5"/>
+      <c r="CS147" s="4"/>
     </row>
     <row r="148" spans="97:97">
-      <c r="CS148" s="5"/>
+      <c r="CS148" s="4"/>
     </row>
     <row r="149" spans="97:97">
-      <c r="CS149" s="5"/>
+      <c r="CS149" s="4"/>
     </row>
     <row r="150" spans="97:97">
-      <c r="CS150" s="5"/>
+      <c r="CS150" s="4"/>
     </row>
     <row r="151" spans="97:97">
-      <c r="CS151" s="5"/>
+      <c r="CS151" s="4"/>
     </row>
     <row r="152" spans="97:97">
-      <c r="CS152" s="5"/>
+      <c r="CS152" s="4"/>
     </row>
     <row r="153" spans="97:97">
-      <c r="CS153" s="5"/>
+      <c r="CS153" s="4"/>
     </row>
     <row r="154" spans="97:97">
-      <c r="CS154" s="5"/>
+      <c r="CS154" s="4"/>
     </row>
     <row r="155" spans="97:97">
-      <c r="CS155" s="5"/>
+      <c r="CS155" s="4"/>
     </row>
     <row r="156" spans="97:97">
-      <c r="CS156" s="5"/>
+      <c r="CS156" s="4"/>
     </row>
     <row r="157" spans="97:97">
-      <c r="CS157" s="5"/>
+      <c r="CS157" s="4"/>
     </row>
     <row r="158" spans="97:97">
-      <c r="CS158" s="5"/>
+      <c r="CS158" s="4"/>
     </row>
     <row r="159" spans="97:97">
-      <c r="CS159" s="5"/>
+      <c r="CS159" s="4"/>
     </row>
     <row r="160" spans="97:97">
-      <c r="CS160" s="5"/>
+      <c r="CS160" s="4"/>
     </row>
     <row r="161" spans="97:97">
-      <c r="CS161" s="5"/>
+      <c r="CS161" s="4"/>
     </row>
     <row r="162" spans="97:97">
-      <c r="CS162" s="5"/>
+      <c r="CS162" s="4"/>
     </row>
     <row r="163" spans="97:97">
-      <c r="CS163" s="5"/>
+      <c r="CS163" s="4"/>
     </row>
     <row r="164" spans="97:97">
-      <c r="CS164" s="5"/>
+      <c r="CS164" s="4"/>
     </row>
     <row r="165" spans="97:97">
-      <c r="CS165" s="5"/>
+      <c r="CS165" s="4"/>
     </row>
     <row r="166" spans="97:97">
-      <c r="CS166" s="5"/>
+      <c r="CS166" s="4"/>
     </row>
     <row r="167" spans="97:97">
-      <c r="CS167" s="5"/>
+      <c r="CS167" s="4"/>
     </row>
     <row r="168" spans="97:97">
-      <c r="CS168" s="5"/>
+      <c r="CS168" s="4"/>
     </row>
     <row r="169" spans="97:97">
-      <c r="CS169" s="5"/>
+      <c r="CS169" s="4"/>
     </row>
     <row r="170" spans="97:97">
-      <c r="CS170" s="5"/>
+      <c r="CS170" s="4"/>
     </row>
     <row r="171" spans="97:97">
-      <c r="CS171" s="5"/>
+      <c r="CS171" s="4"/>
     </row>
     <row r="172" spans="97:97">
-      <c r="CS172" s="5"/>
+      <c r="CS172" s="4"/>
     </row>
     <row r="173" spans="97:97">
-      <c r="CS173" s="5"/>
+      <c r="CS173" s="4"/>
     </row>
     <row r="174" spans="97:97">
-      <c r="CS174" s="5"/>
+      <c r="CS174" s="4"/>
     </row>
     <row r="175" spans="97:97">
-      <c r="CS175" s="5"/>
+      <c r="CS175" s="4"/>
     </row>
     <row r="176" spans="97:97">
-      <c r="CS176" s="5"/>
+      <c r="CS176" s="4"/>
     </row>
     <row r="177" spans="97:97">
-      <c r="CS177" s="5"/>
+      <c r="CS177" s="4"/>
     </row>
     <row r="178" spans="97:97">
-      <c r="CS178" s="5"/>
+      <c r="CS178" s="4"/>
     </row>
     <row r="179" spans="97:97">
-      <c r="CS179" s="5"/>
+      <c r="CS179" s="4"/>
     </row>
     <row r="180" spans="97:97">
-      <c r="CS180" s="5"/>
+      <c r="CS180" s="4"/>
     </row>
     <row r="181" spans="97:97">
-      <c r="CS181" s="5"/>
+      <c r="CS181" s="4"/>
     </row>
     <row r="182" spans="97:97">
-      <c r="CS182" s="5"/>
+      <c r="CS182" s="4"/>
     </row>
     <row r="183" spans="97:97">
-      <c r="CS183" s="5"/>
+      <c r="CS183" s="4"/>
     </row>
     <row r="184" spans="97:97">
-      <c r="CS184" s="5"/>
+      <c r="CS184" s="4"/>
     </row>
     <row r="185" spans="97:97">
-      <c r="CS185" s="5"/>
+      <c r="CS185" s="4"/>
     </row>
     <row r="186" spans="97:97">
-      <c r="CS186" s="5"/>
+      <c r="CS186" s="4"/>
     </row>
     <row r="187" spans="97:97">
-      <c r="CS187" s="5"/>
+      <c r="CS187" s="4"/>
     </row>
     <row r="188" spans="97:97">
-      <c r="CS188" s="5"/>
+      <c r="CS188" s="4"/>
     </row>
     <row r="189" spans="97:97">
-      <c r="CS189" s="5"/>
+      <c r="CS189" s="4"/>
     </row>
     <row r="190" spans="97:97">
-      <c r="CS190" s="5"/>
+      <c r="CS190" s="4"/>
     </row>
     <row r="191" spans="97:97">
-      <c r="CS191" s="5"/>
+      <c r="CS191" s="4"/>
     </row>
     <row r="192" spans="97:97">
-      <c r="CS192" s="5"/>
+      <c r="CS192" s="4"/>
     </row>
     <row r="193" spans="97:97">
-      <c r="CS193" s="5"/>
+      <c r="CS193" s="4"/>
     </row>
     <row r="194" spans="97:97">
-      <c r="CS194" s="5"/>
+      <c r="CS194" s="4"/>
     </row>
     <row r="195" spans="97:97">
-      <c r="CS195" s="5"/>
+      <c r="CS195" s="4"/>
     </row>
     <row r="196" spans="97:97">
-      <c r="CS196" s="5"/>
+      <c r="CS196" s="4"/>
     </row>
     <row r="197" spans="97:97">
-      <c r="CS197" s="5"/>
+      <c r="CS197" s="4"/>
     </row>
     <row r="198" spans="97:97">
-      <c r="CS198" s="5"/>
+      <c r="CS198" s="4"/>
     </row>
     <row r="199" spans="97:97">
-      <c r="CS199" s="5"/>
+      <c r="CS199" s="4"/>
     </row>
     <row r="200" spans="97:97">
-      <c r="CS200" s="5"/>
+      <c r="CS200" s="4"/>
     </row>
     <row r="201" spans="97:97">
-      <c r="CS201" s="5"/>
+      <c r="CS201" s="4"/>
     </row>
     <row r="202" spans="97:97">
-      <c r="CS202" s="5"/>
+      <c r="CS202" s="4"/>
     </row>
     <row r="203" spans="97:97">
-      <c r="CS203" s="5"/>
+      <c r="CS203" s="4"/>
     </row>
     <row r="204" spans="97:97">
-      <c r="CS204" s="5"/>
+      <c r="CS204" s="4"/>
     </row>
     <row r="205" spans="97:97">
-      <c r="CS205" s="5"/>
+      <c r="CS205" s="4"/>
     </row>
     <row r="206" spans="97:97">
-      <c r="CS206" s="5"/>
+      <c r="CS206" s="4"/>
     </row>
     <row r="207" spans="97:97">
-      <c r="CS207" s="5"/>
+      <c r="CS207" s="4"/>
     </row>
     <row r="208" spans="97:97">
-      <c r="CS208" s="5"/>
+      <c r="CS208" s="4"/>
     </row>
     <row r="209" spans="97:97">
-      <c r="CS209" s="5"/>
+      <c r="CS209" s="4"/>
     </row>
     <row r="210" spans="97:97">
-      <c r="CS210" s="5"/>
+      <c r="CS210" s="4"/>
     </row>
     <row r="211" spans="97:97">
-      <c r="CS211" s="5"/>
+      <c r="CS211" s="4"/>
     </row>
     <row r="212" spans="97:97">
-      <c r="CS212" s="5"/>
+      <c r="CS212" s="4"/>
     </row>
     <row r="213" spans="97:97">
-      <c r="CS213" s="5"/>
+      <c r="CS213" s="4"/>
     </row>
     <row r="214" spans="97:97">
-      <c r="CS214" s="5"/>
+      <c r="CS214" s="4"/>
     </row>
     <row r="215" spans="97:97">
-      <c r="CS215" s="5"/>
+      <c r="CS215" s="4"/>
     </row>
     <row r="216" spans="97:97">
-      <c r="CS216" s="5"/>
+      <c r="CS216" s="4"/>
     </row>
     <row r="217" spans="97:97">
-      <c r="CS217" s="5"/>
+      <c r="CS217" s="4"/>
     </row>
     <row r="218" spans="97:97">
-      <c r="CS218" s="5"/>
+      <c r="CS218" s="4"/>
     </row>
     <row r="219" spans="97:97">
-      <c r="CS219" s="5"/>
+      <c r="CS219" s="4"/>
     </row>
     <row r="220" spans="97:97">
-      <c r="CS220" s="5"/>
+      <c r="CS220" s="4"/>
     </row>
     <row r="221" spans="97:97">
-      <c r="CS221" s="5"/>
+      <c r="CS221" s="4"/>
     </row>
     <row r="222" spans="97:97">
-      <c r="CS222" s="5"/>
+      <c r="CS222" s="4"/>
     </row>
     <row r="223" spans="97:97">
-      <c r="CS223" s="5"/>
+      <c r="CS223" s="4"/>
     </row>
     <row r="224" spans="97:97">
-      <c r="CS224" s="5"/>
+      <c r="CS224" s="4"/>
     </row>
     <row r="225" spans="97:97">
-      <c r="CS225" s="5"/>
+      <c r="CS225" s="4"/>
     </row>
     <row r="226" spans="97:97">
-      <c r="CS226" s="5"/>
+      <c r="CS226" s="4"/>
     </row>
     <row r="227" spans="97:97">
-      <c r="CS227" s="5"/>
+      <c r="CS227" s="4"/>
     </row>
     <row r="228" spans="97:97">
-      <c r="CS228" s="5"/>
+      <c r="CS228" s="4"/>
     </row>
     <row r="229" spans="97:97">
-      <c r="CS229" s="5"/>
+      <c r="CS229" s="4"/>
     </row>
     <row r="230" spans="97:97">
-      <c r="CS230" s="5"/>
+      <c r="CS230" s="4"/>
     </row>
     <row r="231" spans="97:97">
-      <c r="CS231" s="5"/>
+      <c r="CS231" s="4"/>
     </row>
     <row r="232" spans="97:97">
-      <c r="CS232" s="5"/>
+      <c r="CS232" s="4"/>
     </row>
     <row r="233" spans="97:97">
-      <c r="CS233" s="5"/>
+      <c r="CS233" s="4"/>
     </row>
     <row r="234" spans="97:97">
-      <c r="CS234" s="5"/>
+      <c r="CS234" s="4"/>
     </row>
     <row r="235" spans="97:97">
-      <c r="CS235" s="5"/>
+      <c r="CS235" s="4"/>
     </row>
     <row r="236" spans="97:97">
-      <c r="CS236" s="5"/>
+      <c r="CS236" s="4"/>
     </row>
     <row r="237" spans="97:97">
-      <c r="CS237" s="5"/>
+      <c r="CS237" s="4"/>
     </row>
     <row r="238" spans="97:97">
-      <c r="CS238" s="5"/>
+      <c r="CS238" s="4"/>
     </row>
     <row r="239" spans="97:97">
-      <c r="CS239" s="5"/>
+      <c r="CS239" s="4"/>
     </row>
     <row r="240" spans="97:97">
-      <c r="CS240" s="5"/>
+      <c r="CS240" s="4"/>
     </row>
     <row r="241" spans="97:97">
-      <c r="CS241" s="5"/>
+      <c r="CS241" s="4"/>
     </row>
     <row r="242" spans="97:97">
-      <c r="CS242" s="5"/>
+      <c r="CS242" s="4"/>
     </row>
     <row r="243" spans="97:97">
-      <c r="CS243" s="5"/>
+      <c r="CS243" s="4"/>
     </row>
     <row r="244" spans="97:97">
-      <c r="CS244" s="5"/>
+      <c r="CS244" s="4"/>
     </row>
     <row r="245" spans="97:97">
-      <c r="CS245" s="5"/>
+      <c r="CS245" s="4"/>
     </row>
     <row r="246" spans="97:97">
-      <c r="CS246" s="5"/>
+      <c r="CS246" s="4"/>
     </row>
     <row r="247" spans="97:97">
-      <c r="CS247" s="5"/>
+      <c r="CS247" s="4"/>
     </row>
     <row r="248" spans="97:97">
-      <c r="CS248" s="5"/>
+      <c r="CS248" s="4"/>
     </row>
     <row r="249" spans="97:97">
-      <c r="CS249" s="5"/>
+      <c r="CS249" s="4"/>
     </row>
     <row r="250" spans="97:97">
-      <c r="CS250" s="5"/>
+      <c r="CS250" s="4"/>
     </row>
     <row r="251" spans="97:97">
-      <c r="CS251" s="5"/>
+      <c r="CS251" s="4"/>
     </row>
     <row r="252" spans="97:97">
-      <c r="CS252" s="5"/>
+      <c r="CS252" s="4"/>
     </row>
     <row r="253" spans="97:97">
-      <c r="CS253" s="5"/>
+      <c r="CS253" s="4"/>
     </row>
     <row r="254" spans="97:97">
-      <c r="CS254" s="5"/>
+      <c r="CS254" s="4"/>
     </row>
     <row r="255" spans="97:97">
-      <c r="CS255" s="5"/>
+      <c r="CS255" s="4"/>
     </row>
     <row r="256" spans="97:97">
-      <c r="CS256" s="5"/>
+      <c r="CS256" s="4"/>
     </row>
     <row r="257" spans="97:97">
-      <c r="CS257" s="5"/>
+      <c r="CS257" s="4"/>
     </row>
     <row r="258" spans="97:97">
-      <c r="CS258" s="5"/>
+      <c r="CS258" s="4"/>
     </row>
     <row r="259" spans="97:97">
-      <c r="CS259" s="5"/>
+      <c r="CS259" s="4"/>
     </row>
     <row r="260" spans="97:97">
-      <c r="CS260" s="5"/>
+      <c r="CS260" s="4"/>
     </row>
     <row r="261" spans="97:97">
-      <c r="CS261" s="5"/>
+      <c r="CS261" s="4"/>
     </row>
     <row r="262" spans="97:97">
-      <c r="CS262" s="5"/>
+      <c r="CS262" s="4"/>
     </row>
     <row r="263" spans="97:97">
-      <c r="CS263" s="5"/>
+      <c r="CS263" s="4"/>
     </row>
     <row r="264" spans="97:97">
-      <c r="CS264" s="5"/>
+      <c r="CS264" s="4"/>
     </row>
     <row r="265" spans="97:97">
-      <c r="CS265" s="5"/>
+      <c r="CS265" s="4"/>
     </row>
     <row r="266" spans="97:97">
-      <c r="CS266" s="5"/>
+      <c r="CS266" s="4"/>
     </row>
     <row r="267" spans="97:97">
-      <c r="CS267" s="5"/>
+      <c r="CS267" s="4"/>
     </row>
     <row r="268" spans="97:97">
-      <c r="CS268" s="5"/>
+      <c r="CS268" s="4"/>
     </row>
     <row r="269" spans="97:97">
-      <c r="CS269" s="5"/>
+      <c r="CS269" s="4"/>
     </row>
     <row r="270" spans="97:97">
-      <c r="CS270" s="5"/>
+      <c r="CS270" s="4"/>
     </row>
     <row r="271" spans="97:97">
-      <c r="CS271" s="5"/>
+      <c r="CS271" s="4"/>
     </row>
     <row r="272" spans="97:97">
-      <c r="CS272" s="5"/>
+      <c r="CS272" s="4"/>
     </row>
     <row r="273" spans="97:97">
-      <c r="CS273" s="5"/>
+      <c r="CS273" s="4"/>
     </row>
     <row r="274" spans="97:97">
-      <c r="CS274" s="5"/>
+      <c r="CS274" s="4"/>
     </row>
     <row r="275" spans="97:97">
-      <c r="CS275" s="5"/>
+      <c r="CS275" s="4"/>
     </row>
     <row r="276" spans="97:97">
-      <c r="CS276" s="5"/>
+      <c r="CS276" s="4"/>
     </row>
     <row r="277" spans="97:97">
-      <c r="CS277" s="5"/>
+      <c r="CS277" s="4"/>
     </row>
     <row r="278" spans="97:97">
-      <c r="CS278" s="5"/>
+      <c r="CS278" s="4"/>
     </row>
     <row r="279" spans="97:97">
-      <c r="CS279" s="5"/>
+      <c r="CS279" s="4"/>
     </row>
     <row r="280" spans="97:97">
-      <c r="CS280" s="5"/>
+      <c r="CS280" s="4"/>
     </row>
     <row r="281" spans="97:97">
-      <c r="CS281" s="5"/>
+      <c r="CS281" s="4"/>
     </row>
     <row r="282" spans="97:97">
-      <c r="CS282" s="5"/>
+      <c r="CS282" s="4"/>
     </row>
     <row r="283" spans="97:97">
-      <c r="CS283" s="5"/>
+      <c r="CS283" s="4"/>
     </row>
     <row r="284" spans="97:97">
-      <c r="CS284" s="5"/>
+      <c r="CS284" s="4"/>
     </row>
     <row r="285" spans="97:97">
-      <c r="CS285" s="5"/>
+      <c r="CS285" s="4"/>
     </row>
     <row r="286" spans="97:97">
-      <c r="CS286" s="5"/>
+      <c r="CS286" s="4"/>
     </row>
     <row r="287" spans="97:97">
-      <c r="CS287" s="5"/>
+      <c r="CS287" s="4"/>
     </row>
     <row r="288" spans="97:97">
-      <c r="CS288" s="5"/>
+      <c r="CS288" s="4"/>
     </row>
     <row r="289" spans="97:97">
-      <c r="CS289" s="5"/>
+      <c r="CS289" s="4"/>
     </row>
     <row r="290" spans="97:97">
-      <c r="CS290" s="5"/>
+      <c r="CS290" s="4"/>
     </row>
     <row r="291" spans="97:97">
-      <c r="CS291" s="5"/>
+      <c r="CS291" s="4"/>
     </row>
     <row r="292" spans="97:97">
-      <c r="CS292" s="5"/>
+      <c r="CS292" s="4"/>
     </row>
     <row r="293" spans="97:97">
-      <c r="CS293" s="5"/>
+      <c r="CS293" s="4"/>
     </row>
     <row r="294" spans="97:97">
-      <c r="CS294" s="5"/>
+      <c r="CS294" s="4"/>
     </row>
     <row r="295" spans="97:97">
-      <c r="CS295" s="5"/>
+      <c r="CS295" s="4"/>
     </row>
     <row r="296" spans="97:97">
-      <c r="CS296" s="5"/>
+      <c r="CS296" s="4"/>
     </row>
     <row r="297" spans="97:97">
-      <c r="CS297" s="5"/>
+      <c r="CS297" s="4"/>
     </row>
     <row r="298" spans="97:97">
-      <c r="CS298" s="5"/>
+      <c r="CS298" s="4"/>
     </row>
     <row r="299" spans="97:97">
-      <c r="CS299" s="5"/>
+      <c r="CS299" s="4"/>
     </row>
     <row r="300" spans="97:97">
-      <c r="CS300" s="5"/>
+      <c r="CS300" s="4"/>
     </row>
     <row r="301" spans="97:97">
-      <c r="CS301" s="5"/>
+      <c r="CS301" s="4"/>
     </row>
     <row r="302" spans="97:97">
-      <c r="CS302" s="5"/>
+      <c r="CS302" s="4"/>
     </row>
     <row r="303" spans="97:97">
-      <c r="CS303" s="5"/>
+      <c r="CS303" s="4"/>
     </row>
     <row r="304" spans="97:97">
-      <c r="CS304" s="5"/>
+      <c r="CS304" s="4"/>
     </row>
     <row r="305" spans="97:97">
-      <c r="CS305" s="5"/>
+      <c r="CS305" s="4"/>
     </row>
     <row r="306" spans="97:97">
-      <c r="CS306" s="5"/>
+      <c r="CS306" s="4"/>
     </row>
     <row r="307" spans="97:97">
-      <c r="CS307" s="5"/>
+      <c r="CS307" s="4"/>
     </row>
     <row r="308" spans="97:97">
-      <c r="CS308" s="5"/>
+      <c r="CS308" s="4"/>
     </row>
     <row r="309" spans="97:97">
-      <c r="CS309" s="5"/>
+      <c r="CS309" s="4"/>
     </row>
     <row r="310" spans="97:97">
-      <c r="CS310" s="5"/>
+      <c r="CS310" s="4"/>
     </row>
     <row r="311" spans="97:97">
-      <c r="CS311" s="5"/>
+      <c r="CS311" s="4"/>
     </row>
     <row r="312" spans="97:97">
-      <c r="CS312" s="5"/>
+      <c r="CS312" s="4"/>
     </row>
     <row r="313" spans="97:97">
-      <c r="CS313" s="5"/>
+      <c r="CS313" s="4"/>
     </row>
     <row r="314" spans="97:97">
-      <c r="CS314" s="5"/>
+      <c r="CS314" s="4"/>
     </row>
     <row r="315" spans="97:97">
-      <c r="CS315" s="5"/>
+      <c r="CS315" s="4"/>
     </row>
     <row r="316" spans="97:97">
-      <c r="CS316" s="5"/>
+      <c r="CS316" s="4"/>
     </row>
     <row r="317" spans="97:97">
-      <c r="CS317" s="5"/>
+      <c r="CS317" s="4"/>
     </row>
     <row r="318" spans="97:97">
-      <c r="CS318" s="5"/>
+      <c r="CS318" s="4"/>
     </row>
     <row r="319" spans="97:97">
-      <c r="CS319" s="5"/>
+      <c r="CS319" s="4"/>
     </row>
     <row r="320" spans="97:97">
-      <c r="CS320" s="5"/>
+      <c r="CS320" s="4"/>
     </row>
     <row r="321" spans="97:97">
-      <c r="CS321" s="5"/>
+      <c r="CS321" s="4"/>
     </row>
     <row r="322" spans="97:97">
-      <c r="CS322" s="5"/>
+      <c r="CS322" s="4"/>
     </row>
     <row r="323" spans="97:97">
-      <c r="CS323" s="5"/>
+      <c r="CS323" s="4"/>
     </row>
     <row r="324" spans="97:97">
-      <c r="CS324" s="5"/>
+      <c r="CS324" s="4"/>
     </row>
     <row r="325" spans="97:97">
-      <c r="CS325" s="5"/>
+      <c r="CS325" s="4"/>
     </row>
     <row r="326" spans="97:97">
-      <c r="CS326" s="5"/>
+      <c r="CS326" s="4"/>
     </row>
     <row r="327" spans="97:97">
-      <c r="CS327" s="5"/>
+      <c r="CS327" s="4"/>
     </row>
     <row r="328" spans="97:97">
-      <c r="CS328" s="5"/>
+      <c r="CS328" s="4"/>
     </row>
     <row r="329" spans="97:97">
-      <c r="CS329" s="5"/>
+      <c r="CS329" s="4"/>
     </row>
     <row r="330" spans="97:97">
-      <c r="CS330" s="5"/>
+      <c r="CS330" s="4"/>
     </row>
     <row r="331" spans="97:97">
-      <c r="CS331" s="5"/>
+      <c r="CS331" s="4"/>
     </row>
     <row r="332" spans="97:97">
-      <c r="CS332" s="5"/>
+      <c r="CS332" s="4"/>
     </row>
     <row r="333" spans="97:97">
-      <c r="CS333" s="5"/>
+      <c r="CS333" s="4"/>
     </row>
     <row r="334" spans="97:97">
-      <c r="CS334" s="5"/>
+      <c r="CS334" s="4"/>
     </row>
     <row r="335" spans="97:97">
-      <c r="CS335" s="5"/>
+      <c r="CS335" s="4"/>
     </row>
     <row r="336" spans="97:97">
-      <c r="CS336" s="5"/>
+      <c r="CS336" s="4"/>
     </row>
     <row r="337" spans="97:97">
-      <c r="CS337" s="5"/>
+      <c r="CS337" s="4"/>
     </row>
     <row r="338" spans="97:97">
-      <c r="CS338" s="5"/>
+      <c r="CS338" s="4"/>
     </row>
     <row r="339" spans="97:97">
-      <c r="CS339" s="5"/>
+      <c r="CS339" s="4"/>
     </row>
     <row r="340" spans="97:97">
-      <c r="CS340" s="5"/>
+      <c r="CS340" s="4"/>
     </row>
     <row r="341" spans="97:97">
-      <c r="CS341" s="5"/>
+      <c r="CS341" s="4"/>
     </row>
     <row r="342" spans="97:97">
-      <c r="CS342" s="5"/>
+      <c r="CS342" s="4"/>
     </row>
     <row r="343" spans="97:97">
-      <c r="CS343" s="5"/>
+      <c r="CS343" s="4"/>
     </row>
     <row r="344" spans="97:97">
-      <c r="CS344" s="5"/>
+      <c r="CS344" s="4"/>
     </row>
     <row r="345" spans="97:97">
-      <c r="CS345" s="5"/>
+      <c r="CS345" s="4"/>
     </row>
     <row r="346" spans="97:97">
-      <c r="CS346" s="5"/>
+      <c r="CS346" s="4"/>
     </row>
     <row r="347" spans="97:97">
-      <c r="CS347" s="5"/>
+      <c r="CS347" s="4"/>
     </row>
     <row r="348" spans="97:97">
-      <c r="CS348" s="5"/>
+      <c r="CS348" s="4"/>
     </row>
     <row r="349" spans="97:97">
-      <c r="CS349" s="5"/>
+      <c r="CS349" s="4"/>
     </row>
     <row r="350" spans="97:97">
-      <c r="CS350" s="5"/>
+      <c r="CS350" s="4"/>
     </row>
     <row r="351" spans="97:97">
-      <c r="CS351" s="5"/>
+      <c r="CS351" s="4"/>
     </row>
     <row r="352" spans="97:97">
-      <c r="CS352" s="5"/>
+      <c r="CS352" s="4"/>
     </row>
     <row r="353" spans="97:97">
-      <c r="CS353" s="5"/>
+      <c r="CS353" s="4"/>
     </row>
     <row r="354" spans="97:97">
-      <c r="CS354" s="5"/>
+      <c r="CS354" s="4"/>
     </row>
     <row r="355" spans="97:97">
-      <c r="CS355" s="5"/>
+      <c r="CS355" s="4"/>
     </row>
     <row r="356" spans="97:97">
-      <c r="CS356" s="5"/>
+      <c r="CS356" s="4"/>
     </row>
     <row r="357" spans="97:97">
-      <c r="CS357" s="5"/>
+      <c r="CS357" s="4"/>
     </row>
     <row r="358" spans="97:97">
-      <c r="CS358" s="5"/>
+      <c r="CS358" s="4"/>
     </row>
     <row r="359" spans="97:97">
-      <c r="CS359" s="5"/>
+      <c r="CS359" s="4"/>
     </row>
     <row r="360" spans="97:97">
-      <c r="CS360" s="5"/>
+      <c r="CS360" s="4"/>
     </row>
     <row r="361" spans="97:97">
-      <c r="CS361" s="5"/>
+      <c r="CS361" s="4"/>
     </row>
     <row r="362" spans="97:97">
-      <c r="CS362" s="5"/>
+      <c r="CS362" s="4"/>
     </row>
     <row r="363" spans="97:97">
-      <c r="CS363" s="5"/>
+      <c r="CS363" s="4"/>
     </row>
     <row r="364" spans="97:97">
-      <c r="CS364" s="5"/>
+      <c r="CS364" s="4"/>
     </row>
     <row r="365" spans="97:97">
-      <c r="CS365" s="5"/>
+      <c r="CS365" s="4"/>
     </row>
     <row r="366" spans="97:97">
-      <c r="CS366" s="5"/>
+      <c r="CS366" s="4"/>
     </row>
     <row r="367" spans="97:97">
-      <c r="CS367" s="5"/>
+      <c r="CS367" s="4"/>
     </row>
     <row r="368" spans="97:97">
-      <c r="CS368" s="5"/>
+      <c r="CS368" s="4"/>
     </row>
     <row r="369" spans="97:97">
-      <c r="CS369" s="5"/>
+      <c r="CS369" s="4"/>
     </row>
     <row r="370" spans="97:97">
-      <c r="CS370" s="5"/>
+      <c r="CS370" s="4"/>
     </row>
     <row r="371" spans="97:97">
-      <c r="CS371" s="5"/>
+      <c r="CS371" s="4"/>
     </row>
     <row r="372" spans="97:97">
-      <c r="CS372" s="5"/>
+      <c r="CS372" s="4"/>
     </row>
     <row r="373" spans="97:97">
-      <c r="CS373" s="5"/>
+      <c r="CS373" s="4"/>
     </row>
     <row r="374" spans="97:97">
-      <c r="CS374" s="5"/>
+      <c r="CS374" s="4"/>
     </row>
     <row r="375" spans="97:97">
-      <c r="CS375" s="5"/>
+      <c r="CS375" s="4"/>
     </row>
     <row r="376" spans="97:97">
-      <c r="CS376" s="5"/>
+      <c r="CS376" s="4"/>
     </row>
     <row r="377" spans="97:97">
-      <c r="CS377" s="5"/>
+      <c r="CS377" s="4"/>
     </row>
     <row r="378" spans="97:97">
-      <c r="CS378" s="5"/>
+      <c r="CS378" s="4"/>
     </row>
     <row r="379" spans="97:97">
-      <c r="CS379" s="5"/>
+      <c r="CS379" s="4"/>
     </row>
     <row r="380" spans="97:97">
-      <c r="CS380" s="5"/>
+      <c r="CS380" s="4"/>
     </row>
     <row r="381" spans="97:97">
-      <c r="CS381" s="5"/>
+      <c r="CS381" s="4"/>
     </row>
     <row r="382" spans="97:97">
-      <c r="CS382" s="5"/>
+      <c r="CS382" s="4"/>
     </row>
     <row r="383" spans="97:97">
-      <c r="CS383" s="5"/>
+      <c r="CS383" s="4"/>
     </row>
     <row r="384" spans="97:97">
-      <c r="CS384" s="5"/>
+      <c r="CS384" s="4"/>
     </row>
     <row r="385" spans="97:97">
-      <c r="CS385" s="5"/>
+      <c r="CS385" s="4"/>
     </row>
     <row r="386" spans="97:97">
-      <c r="CS386" s="5"/>
+      <c r="CS386" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3568,7 +3557,7 @@
       <c r="B2" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>195</v>
       </c>
       <c r="D2" t="s">
@@ -3603,7 +3592,7 @@
       <c r="B3" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>196</v>
       </c>
       <c r="D3" t="s">

</xml_diff>

<commit_message>
updated calculations to account correctly for pip value and swap
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D82A1F9-B375-594B-8644-B00D0E1D1669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73636B8-C37C-2F4F-B189-9BD9B2EEA286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1526,10 +1526,10 @@
   <dimension ref="A1:CT386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomRight" activeCell="CO9" sqref="CO9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -2017,10 +2017,10 @@
         <v>45</v>
       </c>
       <c r="CS2" s="11">
-        <v>43831</v>
-      </c>
-      <c r="CT2" s="8" t="s">
-        <v>3</v>
+        <v>43101</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:98">
@@ -2030,8 +2030,8 @@
       <c r="B3" t="s">
         <v>204</v>
       </c>
-      <c r="C3" t="s">
-        <v>112</v>
+      <c r="C3" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D3" t="s">
         <v>127</v>
@@ -2165,8 +2165,8 @@
       <c r="CR3">
         <v>45</v>
       </c>
-      <c r="CS3" s="4">
-        <v>43831</v>
+      <c r="CS3" s="11">
+        <v>43101</v>
       </c>
       <c r="CT3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
more swap and profit updaes
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73636B8-C37C-2F4F-B189-9BD9B2EEA286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEB4703-C1B9-6D45-B7BE-64EECC1EF8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1526,10 +1526,10 @@
   <dimension ref="A1:CT386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CO9" sqref="CO9"/>
+      <selection pane="bottomRight" activeCell="CT2" sqref="CT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -1876,7 +1876,7 @@
         <v>126</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
         <v>127</v>
@@ -2031,7 +2031,7 @@
         <v>204</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
         <v>127</v>
@@ -2172,11 +2172,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
-      <c r="A4">
+    <row r="4" spans="1:98" s="8" customFormat="1">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="CS4" s="4"/>
+      <c r="B4" s="9"/>
+      <c r="D4"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="BN4" s="10"/>
+      <c r="BP4" s="10"/>
+      <c r="CS4" s="11"/>
+      <c r="CT4"/>
     </row>
     <row r="5" spans="1:98">
       <c r="A5">
@@ -3394,7 +3404,7 @@
           <x14:formula1>
             <xm:f>validation!$J$2:$J$14</xm:f>
           </x14:formula1>
-          <xm:sqref>BW147:BW1048576 CC2:CC1048576 CI2:CI1048576</xm:sqref>
+          <xm:sqref>BW147:BW1048576 CI2:CI1048576 CC2:CC1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -3406,7 +3416,7 @@
           <x14:formula1>
             <xm:f>validation!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>CP51:CP1048576 L2:M1048576 BN2:BN385 R2:R266 S2:S380 W2:W385 G2:G374 BP2:BP1048576</xm:sqref>
+          <xm:sqref>CP51:CP1048576 R4:R266 S4:S380 BP2:BP1048576 G2:G374 W2:W385 R2:S3 BN2:BN385 L2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
@@ -3418,7 +3428,7 @@
           <x14:formula1>
             <xm:f>validation!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>CH2:CH1048576 CB2:CB1048576</xm:sqref>
+          <xm:sqref>CB2:CB1048576 CH2:CH1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
@@ -3430,7 +3440,7 @@
           <x14:formula1>
             <xm:f>validation!$K$2:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>BY2:CA1048576 CE2:CG1048576 CK2:CM1048576</xm:sqref>
+          <xm:sqref>CK2:CM1048576 CE2:CG1048576 BY2:CA1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
@@ -3448,7 +3458,7 @@
           <x14:formula1>
             <xm:f>validation!$H$2:$H$20</xm:f>
           </x14:formula1>
-          <xm:sqref>BA2:BA1048576 AA2:AA507 AN2:AN507</xm:sqref>
+          <xm:sqref>AN2:AN507 AA2:AA507 BA2:BA1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{66B143F6-674E-F24D-AC17-D3B9F43B9156}">
           <x14:formula1>
@@ -3490,7 +3500,7 @@
           <x14:formula1>
             <xm:f>validation!$I$2:$I$40</xm:f>
           </x14:formula1>
-          <xm:sqref>BB2:BB1048576 AB2:AB507 AO2:AO507</xm:sqref>
+          <xm:sqref>AO2:AO507 AB2:AB507 BB2:BB1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
commit before reversing dates in backtest
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD39A682-1024-5547-9C96-98F96FDE5B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE895B32-2788-A144-9B0F-A8241D5DC732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="207">
   <si>
     <t>strategy_name</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>FakeOut_H</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>GBPUSD</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1529,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -1873,7 +1879,7 @@
         <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -2028,7 +2034,7 @@
         <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>206</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
first rev of updating and optimizing backtest - use of index of time by eurusd and pre reverse the df
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE895B32-2788-A144-9B0F-A8241D5DC732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA312329-37A4-C344-B8A6-70A33365EB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1526,10 +1526,10 @@
   <dimension ref="A1:CT386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="CQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="CR7" sqref="CR7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -2017,7 +2017,7 @@
         <v>45</v>
       </c>
       <c r="CS2" s="4">
-        <v>43101</v>
+        <v>45292</v>
       </c>
       <c r="CT2" t="s">
         <v>3</v>
@@ -2166,7 +2166,7 @@
         <v>45</v>
       </c>
       <c r="CS3" s="4">
-        <v>43101</v>
+        <v>45292</v>
       </c>
       <c r="CT3" t="s">
         <v>7</v>
@@ -3387,7 +3387,7 @@
       <c r="CS386" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>24</formula2>
@@ -3397,7 +3397,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>validation!$J$2:$J$14</xm:f>

</xml_diff>

<commit_message>
new reversed df and time list work
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA312329-37A4-C344-B8A6-70A33365EB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6479AC03-2075-5D43-9BEC-E8F846873A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
   <si>
     <t>strategy_name</t>
   </si>
@@ -651,12 +651,6 @@
   </si>
   <si>
     <t>FakeOut_H</t>
-  </si>
-  <si>
-    <t>EURUSD</t>
-  </si>
-  <si>
-    <t>GBPUSD</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1520,10 @@
   <dimension ref="A1:CT386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CR7" sqref="CR7"/>
+      <selection pane="bottomRight" activeCell="CS3" sqref="CS3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -1879,7 +1873,7 @@
         <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -2017,7 +2011,7 @@
         <v>45</v>
       </c>
       <c r="CS2" s="4">
-        <v>45292</v>
+        <v>43831</v>
       </c>
       <c r="CT2" t="s">
         <v>3</v>
@@ -2034,7 +2028,7 @@
         <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -2166,7 +2160,7 @@
         <v>45</v>
       </c>
       <c r="CS3" s="4">
-        <v>45292</v>
+        <v>43831</v>
       </c>
       <c r="CT3" t="s">
         <v>7</v>
@@ -2176,12 +2170,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="W4" s="5"/>
+      <c r="AK4" s="6"/>
       <c r="BN4" s="5"/>
       <c r="BP4" s="5"/>
       <c r="CS4" s="4"/>
@@ -3387,7 +3376,7 @@
       <c r="CS386" s="4"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>24</formula2>
@@ -3397,12 +3386,12 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="17">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>validation!$J$2:$J$14</xm:f>
           </x14:formula1>
-          <xm:sqref>BW147:BW1048576 CI2:CI1048576 CC2:CC1048576</xm:sqref>
+          <xm:sqref>BW147:BW1048576 CC2:CC1048576 CI2:CI1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -3414,7 +3403,7 @@
           <x14:formula1>
             <xm:f>validation!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>CP51:CP1048576 R4:R266 S4:S380 BP2:BP1048576 G2:G374 W2:W385 R2:S3 BN2:BN385 L2:M1048576</xm:sqref>
+          <xm:sqref>CP51:CP1048576 S5:S380 R2:S4 L2:M1048576 BN2:BN385 W2:W385 G2:G374 BP2:BP1048576 R5:R266</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
@@ -3426,7 +3415,7 @@
           <x14:formula1>
             <xm:f>validation!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>CB2:CB1048576 CH2:CH1048576</xm:sqref>
+          <xm:sqref>CH2:CH1048576 CB2:CB1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
@@ -3438,7 +3427,7 @@
           <x14:formula1>
             <xm:f>validation!$K$2:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>CK2:CM1048576 CE2:CG1048576 BY2:CA1048576</xm:sqref>
+          <xm:sqref>BY2:CA1048576 CE2:CG1048576 CK2:CM1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
@@ -3456,7 +3445,7 @@
           <x14:formula1>
             <xm:f>validation!$H$2:$H$20</xm:f>
           </x14:formula1>
-          <xm:sqref>AN2:AN507 AA2:AA507 BA2:BA1048576</xm:sqref>
+          <xm:sqref>BA2:BA1048576 AA2:AA507 AN2:AN507</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{66B143F6-674E-F24D-AC17-D3B9F43B9156}">
           <x14:formula1>
@@ -3498,7 +3487,7 @@
           <x14:formula1>
             <xm:f>validation!$I$2:$I$40</xm:f>
           </x14:formula1>
-          <xm:sqref>AO2:AO507 AB2:AB507 BB2:BB1048576</xm:sqref>
+          <xm:sqref>BB2:BB1048576 AB2:AB507 AO2:AO507</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
working code for loading pre procssed parquet files
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6479AC03-2075-5D43-9BEC-E8F846873A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9C7A43-26B3-9743-9E8F-93A75872F84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="207">
   <si>
     <t>strategy_name</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>FakeOut_H</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>AUDNZD</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1529,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CS3" sqref="CS3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -1873,7 +1879,7 @@
         <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -2028,7 +2034,7 @@
         <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>206</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
split calculations of indicators and load data - utilize mac for caluclations
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEB31A1-8E55-7D4A-9AEB-1F0DF502C53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C0CB36-013A-3947-BA22-755520E60FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1520,10 +1520,10 @@
   <dimension ref="A1:CT386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="CP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -3501,7 +3501,7 @@
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
rollback - updates made the code slower
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C0CB36-013A-3947-BA22-755520E60FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05A6F05-190C-7046-9E05-D89CBBB725D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="207">
   <si>
     <t>strategy_name</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>FakeOut_H</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>USDJPY</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1529,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="CP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -1873,7 +1879,7 @@
         <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -2011,7 +2017,7 @@
         <v>45</v>
       </c>
       <c r="CS2" s="4">
-        <v>43831</v>
+        <v>45352</v>
       </c>
       <c r="CT2" t="s">
         <v>3</v>
@@ -2028,7 +2034,7 @@
         <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>206</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -2160,7 +2166,7 @@
         <v>45</v>
       </c>
       <c r="CS3" s="4">
-        <v>43831</v>
+        <v>45352</v>
       </c>
       <c r="CT3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
changed tp, sl and trail methods to be prepulated in strategy
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079EA800-7E82-964B-908C-D4BF8BD68C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1B9BB4-1BB8-3E4F-8082-F157F06D361A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="207">
   <si>
     <t>strategy_name</t>
   </si>
@@ -380,9 +380,6 @@
     <t>Marubuzo</t>
   </si>
   <si>
-    <t>trail_both_directions</t>
-  </si>
-  <si>
     <t>UsePerc_Trail</t>
   </si>
   <si>
@@ -657,6 +654,9 @@
   </si>
   <si>
     <t>EURGBP</t>
+  </si>
+  <si>
+    <t>EURGBP;USDJPY</t>
   </si>
 </sst>
 </file>
@@ -1523,13 +1523,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CT386"/>
+  <dimension ref="A1:CS386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="CP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="CP10" sqref="CP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -1548,31 +1548,29 @@
     <col min="14" max="14" width="19.1640625" customWidth="1"/>
     <col min="15" max="15" width="8.1640625" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" customWidth="1"/>
-    <col min="19" max="22" width="9.1640625" customWidth="1"/>
-    <col min="53" max="53" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16.6640625" customWidth="1"/>
-    <col min="67" max="67" width="9.5" customWidth="1"/>
-    <col min="69" max="69" width="10" customWidth="1"/>
-    <col min="70" max="70" width="9.5" customWidth="1"/>
-    <col min="80" max="80" width="10.33203125" customWidth="1"/>
-    <col min="82" max="82" width="11.5" customWidth="1"/>
-    <col min="83" max="83" width="10.5" customWidth="1"/>
-    <col min="84" max="85" width="11" customWidth="1"/>
-    <col min="86" max="86" width="10.5" customWidth="1"/>
-    <col min="87" max="87" width="10.1640625" customWidth="1"/>
-    <col min="88" max="88" width="11.83203125" customWidth="1"/>
-    <col min="89" max="89" width="11.5" customWidth="1"/>
-    <col min="90" max="90" width="10.83203125" customWidth="1"/>
-    <col min="91" max="91" width="10.6640625" customWidth="1"/>
-    <col min="92" max="92" width="12.83203125" customWidth="1"/>
-    <col min="93" max="93" width="13.5" customWidth="1"/>
-    <col min="95" max="95" width="9.6640625" customWidth="1"/>
-    <col min="97" max="97" width="10.6640625" customWidth="1"/>
+    <col min="17" max="21" width="9.1640625" customWidth="1"/>
+    <col min="52" max="52" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.6640625" customWidth="1"/>
+    <col min="66" max="66" width="9.5" customWidth="1"/>
+    <col min="68" max="68" width="10" customWidth="1"/>
+    <col min="69" max="69" width="9.5" customWidth="1"/>
+    <col min="79" max="79" width="10.33203125" customWidth="1"/>
+    <col min="81" max="81" width="11.5" customWidth="1"/>
+    <col min="82" max="82" width="10.5" customWidth="1"/>
+    <col min="83" max="84" width="11" customWidth="1"/>
+    <col min="85" max="85" width="10.5" customWidth="1"/>
+    <col min="86" max="86" width="10.1640625" customWidth="1"/>
+    <col min="87" max="87" width="11.83203125" customWidth="1"/>
+    <col min="88" max="88" width="11.5" customWidth="1"/>
+    <col min="89" max="89" width="10.83203125" customWidth="1"/>
+    <col min="90" max="90" width="10.6640625" customWidth="1"/>
+    <col min="91" max="91" width="12.83203125" customWidth="1"/>
+    <col min="92" max="92" width="13.5" customWidth="1"/>
+    <col min="94" max="94" width="9.6640625" customWidth="1"/>
+    <col min="96" max="96" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="1" customFormat="1" ht="63" customHeight="1">
+    <row r="1" spans="1:97" s="1" customFormat="1" ht="63" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1592,7 +1590,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1625,37 +1623,37 @@
         <v>27</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>141</v>
@@ -1766,120 +1764,117 @@
         <v>176</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>61</v>
+        <v>132</v>
       </c>
       <c r="BR1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BS1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="BT1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BU1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="BV1" s="8" t="s">
-        <v>202</v>
+      <c r="BU1" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="BY1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="CT1" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:98">
+    </row>
+    <row r="2" spans="1:97">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>204</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1888,7 +1883,7 @@
         <v>0.02</v>
       </c>
       <c r="G2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1903,138 +1898,135 @@
         <v>110</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O2">
         <v>10</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0.35</v>
+      </c>
+      <c r="U2">
+        <v>0.25</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="T2">
+      <c r="X2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB2">
+        <v>100</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2">
+        <v>10</v>
+      </c>
+      <c r="AE2">
         <v>1</v>
       </c>
-      <c r="U2">
-        <v>0.35</v>
-      </c>
-      <c r="V2">
-        <v>0.25</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z2">
+      <c r="AF2">
         <v>2</v>
       </c>
-      <c r="AA2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AC2">
-        <v>100</v>
-      </c>
-      <c r="AD2">
+      <c r="AG2">
         <v>3</v>
       </c>
-      <c r="AE2">
-        <v>10</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
+      <c r="AH2">
+        <v>30</v>
+      </c>
+      <c r="AI2">
+        <v>0.1</v>
+      </c>
+      <c r="AJ2">
         <v>2</v>
-      </c>
-      <c r="AH2">
-        <v>3</v>
-      </c>
-      <c r="AI2">
-        <v>30</v>
-      </c>
-      <c r="AJ2">
-        <v>0.1</v>
       </c>
       <c r="AK2">
         <v>2</v>
       </c>
       <c r="AL2">
-        <v>2</v>
-      </c>
-      <c r="AM2">
         <v>0.5</v>
       </c>
-      <c r="BN2" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="BO2">
+      <c r="BM2" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BN2">
         <v>0</v>
       </c>
-      <c r="BP2" s="5" t="s">
-        <v>196</v>
+      <c r="BO2" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BQ2">
+        <v>25</v>
       </c>
       <c r="BR2">
-        <v>25</v>
+        <v>5000</v>
       </c>
       <c r="BS2">
-        <v>5000</v>
+        <v>20</v>
       </c>
       <c r="BT2">
         <v>20</v>
       </c>
       <c r="BU2">
-        <v>20</v>
-      </c>
-      <c r="BV2">
         <v>22</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BV2" t="s">
         <v>67</v>
       </c>
-      <c r="BX2">
+      <c r="BW2">
         <v>1</v>
       </c>
+      <c r="CO2">
+        <v>14</v>
+      </c>
       <c r="CP2">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="CQ2">
         <v>45</v>
       </c>
-      <c r="CR2">
-        <v>45</v>
-      </c>
-      <c r="CS2" s="4">
-        <v>43831</v>
-      </c>
-      <c r="CT2" t="s">
+      <c r="CR2" s="4">
+        <v>45383</v>
+      </c>
+      <c r="CS2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:97">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -2043,7 +2035,7 @@
         <v>0.02</v>
       </c>
       <c r="G3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2058,1340 +2050,1340 @@
         <v>110</v>
       </c>
       <c r="L3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O3">
         <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>196</v>
-      </c>
-      <c r="S3" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
       </c>
       <c r="T3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U3">
         <v>1</v>
       </c>
-      <c r="V3">
+      <c r="V3" t="s">
+        <v>194</v>
+      </c>
+      <c r="W3">
         <v>1</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y3">
+        <v>5</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB3">
+        <v>100</v>
+      </c>
+      <c r="AC3">
+        <v>3</v>
+      </c>
+      <c r="AD3">
+        <v>10</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>2</v>
+      </c>
+      <c r="AG3">
+        <v>3</v>
+      </c>
+      <c r="AH3">
+        <v>30</v>
+      </c>
+      <c r="AI3">
+        <v>0.1</v>
+      </c>
+      <c r="AJ3" s="6">
+        <v>2</v>
+      </c>
+      <c r="AK3">
+        <v>2</v>
+      </c>
+      <c r="AL3">
+        <v>0.5</v>
+      </c>
+      <c r="BM3" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z3">
-        <v>5</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC3">
-        <v>100</v>
-      </c>
-      <c r="AD3">
-        <v>3</v>
-      </c>
-      <c r="AE3">
-        <v>10</v>
-      </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
-        <v>2</v>
-      </c>
-      <c r="AH3">
-        <v>3</v>
-      </c>
-      <c r="AI3">
-        <v>30</v>
-      </c>
-      <c r="AJ3">
-        <v>0.1</v>
-      </c>
-      <c r="AK3" s="6">
-        <v>2</v>
-      </c>
-      <c r="AL3">
-        <v>2</v>
-      </c>
-      <c r="AM3">
-        <v>0.5</v>
-      </c>
-      <c r="BN3" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="BO3">
+      <c r="BN3">
         <v>0</v>
       </c>
-      <c r="BP3" s="5" t="s">
-        <v>196</v>
+      <c r="BO3" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BQ3">
+        <v>25</v>
       </c>
       <c r="BR3">
-        <v>25</v>
+        <v>5000</v>
       </c>
       <c r="BS3">
-        <v>5000</v>
+        <v>20</v>
       </c>
       <c r="BT3">
         <v>20</v>
       </c>
-      <c r="BU3">
-        <v>20</v>
+      <c r="CO3">
+        <v>14</v>
       </c>
       <c r="CP3">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="CQ3">
         <v>45</v>
       </c>
-      <c r="CR3">
-        <v>45</v>
-      </c>
-      <c r="CS3" s="4">
-        <v>43831</v>
-      </c>
-      <c r="CT3" t="s">
+      <c r="CR3" s="4">
+        <v>45383</v>
+      </c>
+      <c r="CS3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:97">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="AK4" s="6"/>
-      <c r="BN4" s="5"/>
-      <c r="BP4" s="5"/>
-      <c r="CS4" s="4"/>
-    </row>
-    <row r="5" spans="1:98">
+      <c r="AJ4" s="6"/>
+      <c r="BM4" s="5"/>
+      <c r="BO4" s="5"/>
+      <c r="CR4" s="4"/>
+    </row>
+    <row r="5" spans="1:97">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="CS5" s="4"/>
-    </row>
-    <row r="6" spans="1:98">
+      <c r="CR5" s="4"/>
+    </row>
+    <row r="6" spans="1:97">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="CS6" s="4"/>
-    </row>
-    <row r="7" spans="1:98">
+      <c r="CR6" s="4"/>
+    </row>
+    <row r="7" spans="1:97">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="CS7" s="4"/>
-    </row>
-    <row r="8" spans="1:98">
+      <c r="CR7" s="4"/>
+    </row>
+    <row r="8" spans="1:97">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="CS8" s="4"/>
-    </row>
-    <row r="9" spans="1:98">
+      <c r="CR8" s="4"/>
+    </row>
+    <row r="9" spans="1:97">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="CS9" s="4"/>
-    </row>
-    <row r="10" spans="1:98">
+      <c r="CR9" s="4"/>
+    </row>
+    <row r="10" spans="1:97">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="CS10" s="4"/>
-    </row>
-    <row r="11" spans="1:98">
+      <c r="CR10" s="4"/>
+    </row>
+    <row r="11" spans="1:97">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="CS11" s="4"/>
-    </row>
-    <row r="12" spans="1:98">
+      <c r="CR11" s="4"/>
+    </row>
+    <row r="12" spans="1:97">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="CS12" s="4"/>
-    </row>
-    <row r="13" spans="1:98">
+      <c r="CR12" s="4"/>
+    </row>
+    <row r="13" spans="1:97">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="CS13" s="4"/>
-    </row>
-    <row r="14" spans="1:98">
+      <c r="CR13" s="4"/>
+    </row>
+    <row r="14" spans="1:97">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="CS14" s="4"/>
-    </row>
-    <row r="15" spans="1:98">
+      <c r="CR14" s="4"/>
+    </row>
+    <row r="15" spans="1:97">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="CS15" s="4"/>
-    </row>
-    <row r="16" spans="1:98">
+      <c r="CR15" s="4"/>
+    </row>
+    <row r="16" spans="1:97">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="CS16" s="4"/>
-    </row>
-    <row r="17" spans="1:97">
+      <c r="CR16" s="4"/>
+    </row>
+    <row r="17" spans="1:96">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="CS17" s="4"/>
-    </row>
-    <row r="18" spans="1:97">
+      <c r="CR17" s="4"/>
+    </row>
+    <row r="18" spans="1:96">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="CS18" s="4"/>
-    </row>
-    <row r="19" spans="1:97">
+      <c r="CR18" s="4"/>
+    </row>
+    <row r="19" spans="1:96">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="CS19" s="4"/>
-    </row>
-    <row r="20" spans="1:97">
+      <c r="CR19" s="4"/>
+    </row>
+    <row r="20" spans="1:96">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="CS20" s="4"/>
-    </row>
-    <row r="21" spans="1:97">
+      <c r="D20" t="s">
+        <v>206</v>
+      </c>
+      <c r="CR20" s="4"/>
+    </row>
+    <row r="21" spans="1:96">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
-      </c>
-      <c r="CS21" s="4">
+        <v>205</v>
+      </c>
+      <c r="CR21" s="4">
         <v>45383</v>
       </c>
     </row>
-    <row r="22" spans="1:97">
+    <row r="22" spans="1:96">
       <c r="D22" t="s">
-        <v>205</v>
-      </c>
-      <c r="CS22" s="4">
+        <v>204</v>
+      </c>
+      <c r="CR22" s="4">
         <v>45383</v>
       </c>
     </row>
-    <row r="23" spans="1:97">
+    <row r="23" spans="1:96">
       <c r="D23" t="s">
-        <v>127</v>
-      </c>
-      <c r="CS23" s="4">
+        <v>126</v>
+      </c>
+      <c r="CR23" s="4">
         <v>43831</v>
       </c>
     </row>
-    <row r="24" spans="1:97">
-      <c r="CS24" s="4"/>
-    </row>
-    <row r="25" spans="1:97">
-      <c r="CS25" s="4"/>
-    </row>
-    <row r="26" spans="1:97">
-      <c r="CS26" s="4"/>
-    </row>
-    <row r="27" spans="1:97">
-      <c r="CS27" s="4"/>
-    </row>
-    <row r="28" spans="1:97">
-      <c r="CS28" s="4"/>
-    </row>
-    <row r="29" spans="1:97">
-      <c r="CS29" s="4"/>
-    </row>
-    <row r="30" spans="1:97">
-      <c r="CS30" s="4"/>
-    </row>
-    <row r="31" spans="1:97">
-      <c r="CS31" s="4"/>
-    </row>
-    <row r="32" spans="1:97">
-      <c r="CS32" s="4"/>
-    </row>
-    <row r="33" spans="97:97">
-      <c r="CS33" s="4"/>
-    </row>
-    <row r="34" spans="97:97">
-      <c r="CS34" s="4"/>
-    </row>
-    <row r="35" spans="97:97">
-      <c r="CS35" s="4"/>
-    </row>
-    <row r="36" spans="97:97">
-      <c r="CS36" s="4"/>
-    </row>
-    <row r="37" spans="97:97">
-      <c r="CS37" s="4"/>
-    </row>
-    <row r="38" spans="97:97">
-      <c r="CS38" s="4"/>
-    </row>
-    <row r="39" spans="97:97">
-      <c r="CS39" s="4"/>
-    </row>
-    <row r="40" spans="97:97">
-      <c r="CS40" s="4"/>
-    </row>
-    <row r="41" spans="97:97">
-      <c r="CS41" s="4"/>
-    </row>
-    <row r="42" spans="97:97">
-      <c r="CS42" s="4"/>
-    </row>
-    <row r="43" spans="97:97">
-      <c r="CS43" s="4"/>
-    </row>
-    <row r="44" spans="97:97">
-      <c r="CS44" s="4"/>
-    </row>
-    <row r="45" spans="97:97">
-      <c r="CS45" s="4"/>
-    </row>
-    <row r="46" spans="97:97">
-      <c r="CS46" s="4"/>
-    </row>
-    <row r="47" spans="97:97">
-      <c r="CS47" s="4"/>
-    </row>
-    <row r="48" spans="97:97">
-      <c r="CS48" s="4"/>
-    </row>
-    <row r="49" spans="97:97">
-      <c r="CS49" s="4"/>
-    </row>
-    <row r="50" spans="97:97">
-      <c r="CS50" s="4"/>
-    </row>
-    <row r="51" spans="97:97">
-      <c r="CS51" s="4"/>
-    </row>
-    <row r="52" spans="97:97">
-      <c r="CS52" s="4"/>
-    </row>
-    <row r="53" spans="97:97">
-      <c r="CS53" s="4"/>
-    </row>
-    <row r="54" spans="97:97">
-      <c r="CS54" s="4"/>
-    </row>
-    <row r="55" spans="97:97">
-      <c r="CS55" s="4"/>
-    </row>
-    <row r="56" spans="97:97">
-      <c r="CS56" s="4"/>
-    </row>
-    <row r="57" spans="97:97">
-      <c r="CS57" s="4"/>
-    </row>
-    <row r="58" spans="97:97">
-      <c r="CS58" s="4"/>
-    </row>
-    <row r="59" spans="97:97">
-      <c r="CS59" s="4"/>
-    </row>
-    <row r="60" spans="97:97">
-      <c r="CS60" s="4"/>
-    </row>
-    <row r="61" spans="97:97">
-      <c r="CS61" s="4"/>
-    </row>
-    <row r="62" spans="97:97">
-      <c r="CS62" s="4"/>
-    </row>
-    <row r="63" spans="97:97">
-      <c r="CS63" s="4"/>
-    </row>
-    <row r="64" spans="97:97">
-      <c r="CS64" s="4"/>
-    </row>
-    <row r="65" spans="97:97">
-      <c r="CS65" s="4"/>
-    </row>
-    <row r="66" spans="97:97">
-      <c r="CS66" s="4"/>
-    </row>
-    <row r="67" spans="97:97">
-      <c r="CS67" s="4"/>
-    </row>
-    <row r="68" spans="97:97">
-      <c r="CS68" s="4"/>
-    </row>
-    <row r="69" spans="97:97">
-      <c r="CS69" s="4"/>
-    </row>
-    <row r="70" spans="97:97">
-      <c r="CS70" s="4"/>
-    </row>
-    <row r="71" spans="97:97">
-      <c r="CS71" s="4"/>
-    </row>
-    <row r="72" spans="97:97">
-      <c r="CS72" s="4"/>
-    </row>
-    <row r="73" spans="97:97">
-      <c r="CS73" s="4"/>
-    </row>
-    <row r="74" spans="97:97">
-      <c r="CS74" s="4"/>
-    </row>
-    <row r="75" spans="97:97">
-      <c r="CS75" s="4"/>
-    </row>
-    <row r="76" spans="97:97">
-      <c r="CS76" s="4"/>
-    </row>
-    <row r="77" spans="97:97">
-      <c r="CS77" s="4"/>
-    </row>
-    <row r="78" spans="97:97">
-      <c r="CS78" s="4"/>
-    </row>
-    <row r="79" spans="97:97">
-      <c r="CS79" s="4"/>
-    </row>
-    <row r="80" spans="97:97">
-      <c r="CS80" s="4"/>
-    </row>
-    <row r="81" spans="97:97">
-      <c r="CS81" s="4"/>
-    </row>
-    <row r="82" spans="97:97">
-      <c r="CS82" s="4"/>
-    </row>
-    <row r="83" spans="97:97">
-      <c r="CS83" s="4"/>
-    </row>
-    <row r="84" spans="97:97">
-      <c r="CS84" s="4"/>
-    </row>
-    <row r="85" spans="97:97">
-      <c r="CS85" s="4"/>
-    </row>
-    <row r="86" spans="97:97">
-      <c r="CS86" s="4"/>
-    </row>
-    <row r="87" spans="97:97">
-      <c r="CS87" s="4"/>
-    </row>
-    <row r="88" spans="97:97">
-      <c r="CS88" s="4"/>
-    </row>
-    <row r="89" spans="97:97">
-      <c r="CS89" s="4"/>
-    </row>
-    <row r="90" spans="97:97">
-      <c r="CS90" s="4"/>
-    </row>
-    <row r="91" spans="97:97">
-      <c r="CS91" s="4"/>
-    </row>
-    <row r="92" spans="97:97">
-      <c r="CS92" s="4"/>
-    </row>
-    <row r="93" spans="97:97">
-      <c r="CS93" s="4"/>
-    </row>
-    <row r="94" spans="97:97">
-      <c r="CS94" s="4"/>
-    </row>
-    <row r="95" spans="97:97">
-      <c r="CS95" s="4"/>
-    </row>
-    <row r="96" spans="97:97">
-      <c r="CS96" s="4"/>
-    </row>
-    <row r="97" spans="97:97">
-      <c r="CS97" s="4"/>
-    </row>
-    <row r="98" spans="97:97">
-      <c r="CS98" s="4"/>
-    </row>
-    <row r="99" spans="97:97">
-      <c r="CS99" s="4"/>
-    </row>
-    <row r="100" spans="97:97">
-      <c r="CS100" s="4"/>
-    </row>
-    <row r="101" spans="97:97">
-      <c r="CS101" s="4"/>
-    </row>
-    <row r="102" spans="97:97">
-      <c r="CS102" s="4"/>
-    </row>
-    <row r="103" spans="97:97">
-      <c r="CS103" s="4"/>
-    </row>
-    <row r="104" spans="97:97">
-      <c r="CS104" s="4"/>
-    </row>
-    <row r="105" spans="97:97">
-      <c r="CS105" s="4"/>
-    </row>
-    <row r="106" spans="97:97">
-      <c r="CS106" s="4"/>
-    </row>
-    <row r="107" spans="97:97">
-      <c r="CS107" s="4"/>
-    </row>
-    <row r="108" spans="97:97">
-      <c r="CS108" s="4"/>
-    </row>
-    <row r="109" spans="97:97">
-      <c r="CS109" s="4"/>
-    </row>
-    <row r="110" spans="97:97">
-      <c r="CS110" s="4"/>
-    </row>
-    <row r="111" spans="97:97">
-      <c r="CS111" s="4"/>
-    </row>
-    <row r="112" spans="97:97">
-      <c r="CS112" s="4"/>
-    </row>
-    <row r="113" spans="97:97">
-      <c r="CS113" s="4"/>
-    </row>
-    <row r="114" spans="97:97">
-      <c r="CS114" s="4"/>
-    </row>
-    <row r="115" spans="97:97">
-      <c r="CS115" s="4"/>
-    </row>
-    <row r="116" spans="97:97">
-      <c r="CS116" s="4"/>
-    </row>
-    <row r="117" spans="97:97">
-      <c r="CS117" s="4"/>
-    </row>
-    <row r="118" spans="97:97">
-      <c r="CS118" s="4"/>
-    </row>
-    <row r="119" spans="97:97">
-      <c r="CS119" s="4"/>
-    </row>
-    <row r="120" spans="97:97">
-      <c r="CS120" s="4"/>
-    </row>
-    <row r="121" spans="97:97">
-      <c r="CS121" s="4"/>
-    </row>
-    <row r="122" spans="97:97">
-      <c r="CS122" s="4"/>
-    </row>
-    <row r="123" spans="97:97">
-      <c r="CS123" s="4"/>
-    </row>
-    <row r="124" spans="97:97">
-      <c r="CS124" s="4"/>
-    </row>
-    <row r="125" spans="97:97">
-      <c r="CS125" s="4"/>
-    </row>
-    <row r="126" spans="97:97">
-      <c r="CS126" s="4"/>
-    </row>
-    <row r="127" spans="97:97">
-      <c r="CS127" s="4"/>
-    </row>
-    <row r="128" spans="97:97">
-      <c r="CS128" s="4"/>
-    </row>
-    <row r="129" spans="97:97">
-      <c r="CS129" s="4"/>
-    </row>
-    <row r="130" spans="97:97">
-      <c r="CS130" s="4"/>
-    </row>
-    <row r="131" spans="97:97">
-      <c r="CS131" s="4"/>
-    </row>
-    <row r="132" spans="97:97">
-      <c r="CS132" s="4"/>
-    </row>
-    <row r="133" spans="97:97">
-      <c r="CS133" s="4"/>
-    </row>
-    <row r="134" spans="97:97">
-      <c r="CS134" s="4"/>
-    </row>
-    <row r="135" spans="97:97">
-      <c r="CS135" s="4"/>
-    </row>
-    <row r="136" spans="97:97">
-      <c r="CS136" s="4"/>
-    </row>
-    <row r="137" spans="97:97">
-      <c r="CS137" s="4"/>
-    </row>
-    <row r="138" spans="97:97">
-      <c r="CS138" s="4"/>
-    </row>
-    <row r="139" spans="97:97">
-      <c r="CS139" s="4"/>
-    </row>
-    <row r="140" spans="97:97">
-      <c r="CS140" s="4"/>
-    </row>
-    <row r="141" spans="97:97">
-      <c r="CS141" s="4"/>
-    </row>
-    <row r="142" spans="97:97">
-      <c r="CS142" s="4"/>
-    </row>
-    <row r="143" spans="97:97">
-      <c r="CS143" s="4"/>
-    </row>
-    <row r="144" spans="97:97">
-      <c r="CS144" s="4"/>
-    </row>
-    <row r="145" spans="97:97">
-      <c r="CS145" s="4"/>
-    </row>
-    <row r="146" spans="97:97">
-      <c r="CS146" s="4"/>
-    </row>
-    <row r="147" spans="97:97">
-      <c r="CS147" s="4"/>
-    </row>
-    <row r="148" spans="97:97">
-      <c r="CS148" s="4"/>
-    </row>
-    <row r="149" spans="97:97">
-      <c r="CS149" s="4"/>
-    </row>
-    <row r="150" spans="97:97">
-      <c r="CS150" s="4"/>
-    </row>
-    <row r="151" spans="97:97">
-      <c r="CS151" s="4"/>
-    </row>
-    <row r="152" spans="97:97">
-      <c r="CS152" s="4"/>
-    </row>
-    <row r="153" spans="97:97">
-      <c r="CS153" s="4"/>
-    </row>
-    <row r="154" spans="97:97">
-      <c r="CS154" s="4"/>
-    </row>
-    <row r="155" spans="97:97">
-      <c r="CS155" s="4"/>
-    </row>
-    <row r="156" spans="97:97">
-      <c r="CS156" s="4"/>
-    </row>
-    <row r="157" spans="97:97">
-      <c r="CS157" s="4"/>
-    </row>
-    <row r="158" spans="97:97">
-      <c r="CS158" s="4"/>
-    </row>
-    <row r="159" spans="97:97">
-      <c r="CS159" s="4"/>
-    </row>
-    <row r="160" spans="97:97">
-      <c r="CS160" s="4"/>
-    </row>
-    <row r="161" spans="97:97">
-      <c r="CS161" s="4"/>
-    </row>
-    <row r="162" spans="97:97">
-      <c r="CS162" s="4"/>
-    </row>
-    <row r="163" spans="97:97">
-      <c r="CS163" s="4"/>
-    </row>
-    <row r="164" spans="97:97">
-      <c r="CS164" s="4"/>
-    </row>
-    <row r="165" spans="97:97">
-      <c r="CS165" s="4"/>
-    </row>
-    <row r="166" spans="97:97">
-      <c r="CS166" s="4"/>
-    </row>
-    <row r="167" spans="97:97">
-      <c r="CS167" s="4"/>
-    </row>
-    <row r="168" spans="97:97">
-      <c r="CS168" s="4"/>
-    </row>
-    <row r="169" spans="97:97">
-      <c r="CS169" s="4"/>
-    </row>
-    <row r="170" spans="97:97">
-      <c r="CS170" s="4"/>
-    </row>
-    <row r="171" spans="97:97">
-      <c r="CS171" s="4"/>
-    </row>
-    <row r="172" spans="97:97">
-      <c r="CS172" s="4"/>
-    </row>
-    <row r="173" spans="97:97">
-      <c r="CS173" s="4"/>
-    </row>
-    <row r="174" spans="97:97">
-      <c r="CS174" s="4"/>
-    </row>
-    <row r="175" spans="97:97">
-      <c r="CS175" s="4"/>
-    </row>
-    <row r="176" spans="97:97">
-      <c r="CS176" s="4"/>
-    </row>
-    <row r="177" spans="97:97">
-      <c r="CS177" s="4"/>
-    </row>
-    <row r="178" spans="97:97">
-      <c r="CS178" s="4"/>
-    </row>
-    <row r="179" spans="97:97">
-      <c r="CS179" s="4"/>
-    </row>
-    <row r="180" spans="97:97">
-      <c r="CS180" s="4"/>
-    </row>
-    <row r="181" spans="97:97">
-      <c r="CS181" s="4"/>
-    </row>
-    <row r="182" spans="97:97">
-      <c r="CS182" s="4"/>
-    </row>
-    <row r="183" spans="97:97">
-      <c r="CS183" s="4"/>
-    </row>
-    <row r="184" spans="97:97">
-      <c r="CS184" s="4"/>
-    </row>
-    <row r="185" spans="97:97">
-      <c r="CS185" s="4"/>
-    </row>
-    <row r="186" spans="97:97">
-      <c r="CS186" s="4"/>
-    </row>
-    <row r="187" spans="97:97">
-      <c r="CS187" s="4"/>
-    </row>
-    <row r="188" spans="97:97">
-      <c r="CS188" s="4"/>
-    </row>
-    <row r="189" spans="97:97">
-      <c r="CS189" s="4"/>
-    </row>
-    <row r="190" spans="97:97">
-      <c r="CS190" s="4"/>
-    </row>
-    <row r="191" spans="97:97">
-      <c r="CS191" s="4"/>
-    </row>
-    <row r="192" spans="97:97">
-      <c r="CS192" s="4"/>
-    </row>
-    <row r="193" spans="97:97">
-      <c r="CS193" s="4"/>
-    </row>
-    <row r="194" spans="97:97">
-      <c r="CS194" s="4"/>
-    </row>
-    <row r="195" spans="97:97">
-      <c r="CS195" s="4"/>
-    </row>
-    <row r="196" spans="97:97">
-      <c r="CS196" s="4"/>
-    </row>
-    <row r="197" spans="97:97">
-      <c r="CS197" s="4"/>
-    </row>
-    <row r="198" spans="97:97">
-      <c r="CS198" s="4"/>
-    </row>
-    <row r="199" spans="97:97">
-      <c r="CS199" s="4"/>
-    </row>
-    <row r="200" spans="97:97">
-      <c r="CS200" s="4"/>
-    </row>
-    <row r="201" spans="97:97">
-      <c r="CS201" s="4"/>
-    </row>
-    <row r="202" spans="97:97">
-      <c r="CS202" s="4"/>
-    </row>
-    <row r="203" spans="97:97">
-      <c r="CS203" s="4"/>
-    </row>
-    <row r="204" spans="97:97">
-      <c r="CS204" s="4"/>
-    </row>
-    <row r="205" spans="97:97">
-      <c r="CS205" s="4"/>
-    </row>
-    <row r="206" spans="97:97">
-      <c r="CS206" s="4"/>
-    </row>
-    <row r="207" spans="97:97">
-      <c r="CS207" s="4"/>
-    </row>
-    <row r="208" spans="97:97">
-      <c r="CS208" s="4"/>
-    </row>
-    <row r="209" spans="97:97">
-      <c r="CS209" s="4"/>
-    </row>
-    <row r="210" spans="97:97">
-      <c r="CS210" s="4"/>
-    </row>
-    <row r="211" spans="97:97">
-      <c r="CS211" s="4"/>
-    </row>
-    <row r="212" spans="97:97">
-      <c r="CS212" s="4"/>
-    </row>
-    <row r="213" spans="97:97">
-      <c r="CS213" s="4"/>
-    </row>
-    <row r="214" spans="97:97">
-      <c r="CS214" s="4"/>
-    </row>
-    <row r="215" spans="97:97">
-      <c r="CS215" s="4"/>
-    </row>
-    <row r="216" spans="97:97">
-      <c r="CS216" s="4"/>
-    </row>
-    <row r="217" spans="97:97">
-      <c r="CS217" s="4"/>
-    </row>
-    <row r="218" spans="97:97">
-      <c r="CS218" s="4"/>
-    </row>
-    <row r="219" spans="97:97">
-      <c r="CS219" s="4"/>
-    </row>
-    <row r="220" spans="97:97">
-      <c r="CS220" s="4"/>
-    </row>
-    <row r="221" spans="97:97">
-      <c r="CS221" s="4"/>
-    </row>
-    <row r="222" spans="97:97">
-      <c r="CS222" s="4"/>
-    </row>
-    <row r="223" spans="97:97">
-      <c r="CS223" s="4"/>
-    </row>
-    <row r="224" spans="97:97">
-      <c r="CS224" s="4"/>
-    </row>
-    <row r="225" spans="97:97">
-      <c r="CS225" s="4"/>
-    </row>
-    <row r="226" spans="97:97">
-      <c r="CS226" s="4"/>
-    </row>
-    <row r="227" spans="97:97">
-      <c r="CS227" s="4"/>
-    </row>
-    <row r="228" spans="97:97">
-      <c r="CS228" s="4"/>
-    </row>
-    <row r="229" spans="97:97">
-      <c r="CS229" s="4"/>
-    </row>
-    <row r="230" spans="97:97">
-      <c r="CS230" s="4"/>
-    </row>
-    <row r="231" spans="97:97">
-      <c r="CS231" s="4"/>
-    </row>
-    <row r="232" spans="97:97">
-      <c r="CS232" s="4"/>
-    </row>
-    <row r="233" spans="97:97">
-      <c r="CS233" s="4"/>
-    </row>
-    <row r="234" spans="97:97">
-      <c r="CS234" s="4"/>
-    </row>
-    <row r="235" spans="97:97">
-      <c r="CS235" s="4"/>
-    </row>
-    <row r="236" spans="97:97">
-      <c r="CS236" s="4"/>
-    </row>
-    <row r="237" spans="97:97">
-      <c r="CS237" s="4"/>
-    </row>
-    <row r="238" spans="97:97">
-      <c r="CS238" s="4"/>
-    </row>
-    <row r="239" spans="97:97">
-      <c r="CS239" s="4"/>
-    </row>
-    <row r="240" spans="97:97">
-      <c r="CS240" s="4"/>
-    </row>
-    <row r="241" spans="97:97">
-      <c r="CS241" s="4"/>
-    </row>
-    <row r="242" spans="97:97">
-      <c r="CS242" s="4"/>
-    </row>
-    <row r="243" spans="97:97">
-      <c r="CS243" s="4"/>
-    </row>
-    <row r="244" spans="97:97">
-      <c r="CS244" s="4"/>
-    </row>
-    <row r="245" spans="97:97">
-      <c r="CS245" s="4"/>
-    </row>
-    <row r="246" spans="97:97">
-      <c r="CS246" s="4"/>
-    </row>
-    <row r="247" spans="97:97">
-      <c r="CS247" s="4"/>
-    </row>
-    <row r="248" spans="97:97">
-      <c r="CS248" s="4"/>
-    </row>
-    <row r="249" spans="97:97">
-      <c r="CS249" s="4"/>
-    </row>
-    <row r="250" spans="97:97">
-      <c r="CS250" s="4"/>
-    </row>
-    <row r="251" spans="97:97">
-      <c r="CS251" s="4"/>
-    </row>
-    <row r="252" spans="97:97">
-      <c r="CS252" s="4"/>
-    </row>
-    <row r="253" spans="97:97">
-      <c r="CS253" s="4"/>
-    </row>
-    <row r="254" spans="97:97">
-      <c r="CS254" s="4"/>
-    </row>
-    <row r="255" spans="97:97">
-      <c r="CS255" s="4"/>
-    </row>
-    <row r="256" spans="97:97">
-      <c r="CS256" s="4"/>
-    </row>
-    <row r="257" spans="97:97">
-      <c r="CS257" s="4"/>
-    </row>
-    <row r="258" spans="97:97">
-      <c r="CS258" s="4"/>
-    </row>
-    <row r="259" spans="97:97">
-      <c r="CS259" s="4"/>
-    </row>
-    <row r="260" spans="97:97">
-      <c r="CS260" s="4"/>
-    </row>
-    <row r="261" spans="97:97">
-      <c r="CS261" s="4"/>
-    </row>
-    <row r="262" spans="97:97">
-      <c r="CS262" s="4"/>
-    </row>
-    <row r="263" spans="97:97">
-      <c r="CS263" s="4"/>
-    </row>
-    <row r="264" spans="97:97">
-      <c r="CS264" s="4"/>
-    </row>
-    <row r="265" spans="97:97">
-      <c r="CS265" s="4"/>
-    </row>
-    <row r="266" spans="97:97">
-      <c r="CS266" s="4"/>
-    </row>
-    <row r="267" spans="97:97">
-      <c r="CS267" s="4"/>
-    </row>
-    <row r="268" spans="97:97">
-      <c r="CS268" s="4"/>
-    </row>
-    <row r="269" spans="97:97">
-      <c r="CS269" s="4"/>
-    </row>
-    <row r="270" spans="97:97">
-      <c r="CS270" s="4"/>
-    </row>
-    <row r="271" spans="97:97">
-      <c r="CS271" s="4"/>
-    </row>
-    <row r="272" spans="97:97">
-      <c r="CS272" s="4"/>
-    </row>
-    <row r="273" spans="97:97">
-      <c r="CS273" s="4"/>
-    </row>
-    <row r="274" spans="97:97">
-      <c r="CS274" s="4"/>
-    </row>
-    <row r="275" spans="97:97">
-      <c r="CS275" s="4"/>
-    </row>
-    <row r="276" spans="97:97">
-      <c r="CS276" s="4"/>
-    </row>
-    <row r="277" spans="97:97">
-      <c r="CS277" s="4"/>
-    </row>
-    <row r="278" spans="97:97">
-      <c r="CS278" s="4"/>
-    </row>
-    <row r="279" spans="97:97">
-      <c r="CS279" s="4"/>
-    </row>
-    <row r="280" spans="97:97">
-      <c r="CS280" s="4"/>
-    </row>
-    <row r="281" spans="97:97">
-      <c r="CS281" s="4"/>
-    </row>
-    <row r="282" spans="97:97">
-      <c r="CS282" s="4"/>
-    </row>
-    <row r="283" spans="97:97">
-      <c r="CS283" s="4"/>
-    </row>
-    <row r="284" spans="97:97">
-      <c r="CS284" s="4"/>
-    </row>
-    <row r="285" spans="97:97">
-      <c r="CS285" s="4"/>
-    </row>
-    <row r="286" spans="97:97">
-      <c r="CS286" s="4"/>
-    </row>
-    <row r="287" spans="97:97">
-      <c r="CS287" s="4"/>
-    </row>
-    <row r="288" spans="97:97">
-      <c r="CS288" s="4"/>
-    </row>
-    <row r="289" spans="97:97">
-      <c r="CS289" s="4"/>
-    </row>
-    <row r="290" spans="97:97">
-      <c r="CS290" s="4"/>
-    </row>
-    <row r="291" spans="97:97">
-      <c r="CS291" s="4"/>
-    </row>
-    <row r="292" spans="97:97">
-      <c r="CS292" s="4"/>
-    </row>
-    <row r="293" spans="97:97">
-      <c r="CS293" s="4"/>
-    </row>
-    <row r="294" spans="97:97">
-      <c r="CS294" s="4"/>
-    </row>
-    <row r="295" spans="97:97">
-      <c r="CS295" s="4"/>
-    </row>
-    <row r="296" spans="97:97">
-      <c r="CS296" s="4"/>
-    </row>
-    <row r="297" spans="97:97">
-      <c r="CS297" s="4"/>
-    </row>
-    <row r="298" spans="97:97">
-      <c r="CS298" s="4"/>
-    </row>
-    <row r="299" spans="97:97">
-      <c r="CS299" s="4"/>
-    </row>
-    <row r="300" spans="97:97">
-      <c r="CS300" s="4"/>
-    </row>
-    <row r="301" spans="97:97">
-      <c r="CS301" s="4"/>
-    </row>
-    <row r="302" spans="97:97">
-      <c r="CS302" s="4"/>
-    </row>
-    <row r="303" spans="97:97">
-      <c r="CS303" s="4"/>
-    </row>
-    <row r="304" spans="97:97">
-      <c r="CS304" s="4"/>
-    </row>
-    <row r="305" spans="97:97">
-      <c r="CS305" s="4"/>
-    </row>
-    <row r="306" spans="97:97">
-      <c r="CS306" s="4"/>
-    </row>
-    <row r="307" spans="97:97">
-      <c r="CS307" s="4"/>
-    </row>
-    <row r="308" spans="97:97">
-      <c r="CS308" s="4"/>
-    </row>
-    <row r="309" spans="97:97">
-      <c r="CS309" s="4"/>
-    </row>
-    <row r="310" spans="97:97">
-      <c r="CS310" s="4"/>
-    </row>
-    <row r="311" spans="97:97">
-      <c r="CS311" s="4"/>
-    </row>
-    <row r="312" spans="97:97">
-      <c r="CS312" s="4"/>
-    </row>
-    <row r="313" spans="97:97">
-      <c r="CS313" s="4"/>
-    </row>
-    <row r="314" spans="97:97">
-      <c r="CS314" s="4"/>
-    </row>
-    <row r="315" spans="97:97">
-      <c r="CS315" s="4"/>
-    </row>
-    <row r="316" spans="97:97">
-      <c r="CS316" s="4"/>
-    </row>
-    <row r="317" spans="97:97">
-      <c r="CS317" s="4"/>
-    </row>
-    <row r="318" spans="97:97">
-      <c r="CS318" s="4"/>
-    </row>
-    <row r="319" spans="97:97">
-      <c r="CS319" s="4"/>
-    </row>
-    <row r="320" spans="97:97">
-      <c r="CS320" s="4"/>
-    </row>
-    <row r="321" spans="97:97">
-      <c r="CS321" s="4"/>
-    </row>
-    <row r="322" spans="97:97">
-      <c r="CS322" s="4"/>
-    </row>
-    <row r="323" spans="97:97">
-      <c r="CS323" s="4"/>
-    </row>
-    <row r="324" spans="97:97">
-      <c r="CS324" s="4"/>
-    </row>
-    <row r="325" spans="97:97">
-      <c r="CS325" s="4"/>
-    </row>
-    <row r="326" spans="97:97">
-      <c r="CS326" s="4"/>
-    </row>
-    <row r="327" spans="97:97">
-      <c r="CS327" s="4"/>
-    </row>
-    <row r="328" spans="97:97">
-      <c r="CS328" s="4"/>
-    </row>
-    <row r="329" spans="97:97">
-      <c r="CS329" s="4"/>
-    </row>
-    <row r="330" spans="97:97">
-      <c r="CS330" s="4"/>
-    </row>
-    <row r="331" spans="97:97">
-      <c r="CS331" s="4"/>
-    </row>
-    <row r="332" spans="97:97">
-      <c r="CS332" s="4"/>
-    </row>
-    <row r="333" spans="97:97">
-      <c r="CS333" s="4"/>
-    </row>
-    <row r="334" spans="97:97">
-      <c r="CS334" s="4"/>
-    </row>
-    <row r="335" spans="97:97">
-      <c r="CS335" s="4"/>
-    </row>
-    <row r="336" spans="97:97">
-      <c r="CS336" s="4"/>
-    </row>
-    <row r="337" spans="97:97">
-      <c r="CS337" s="4"/>
-    </row>
-    <row r="338" spans="97:97">
-      <c r="CS338" s="4"/>
-    </row>
-    <row r="339" spans="97:97">
-      <c r="CS339" s="4"/>
-    </row>
-    <row r="340" spans="97:97">
-      <c r="CS340" s="4"/>
-    </row>
-    <row r="341" spans="97:97">
-      <c r="CS341" s="4"/>
-    </row>
-    <row r="342" spans="97:97">
-      <c r="CS342" s="4"/>
-    </row>
-    <row r="343" spans="97:97">
-      <c r="CS343" s="4"/>
-    </row>
-    <row r="344" spans="97:97">
-      <c r="CS344" s="4"/>
-    </row>
-    <row r="345" spans="97:97">
-      <c r="CS345" s="4"/>
-    </row>
-    <row r="346" spans="97:97">
-      <c r="CS346" s="4"/>
-    </row>
-    <row r="347" spans="97:97">
-      <c r="CS347" s="4"/>
-    </row>
-    <row r="348" spans="97:97">
-      <c r="CS348" s="4"/>
-    </row>
-    <row r="349" spans="97:97">
-      <c r="CS349" s="4"/>
-    </row>
-    <row r="350" spans="97:97">
-      <c r="CS350" s="4"/>
-    </row>
-    <row r="351" spans="97:97">
-      <c r="CS351" s="4"/>
-    </row>
-    <row r="352" spans="97:97">
-      <c r="CS352" s="4"/>
-    </row>
-    <row r="353" spans="97:97">
-      <c r="CS353" s="4"/>
-    </row>
-    <row r="354" spans="97:97">
-      <c r="CS354" s="4"/>
-    </row>
-    <row r="355" spans="97:97">
-      <c r="CS355" s="4"/>
-    </row>
-    <row r="356" spans="97:97">
-      <c r="CS356" s="4"/>
-    </row>
-    <row r="357" spans="97:97">
-      <c r="CS357" s="4"/>
-    </row>
-    <row r="358" spans="97:97">
-      <c r="CS358" s="4"/>
-    </row>
-    <row r="359" spans="97:97">
-      <c r="CS359" s="4"/>
-    </row>
-    <row r="360" spans="97:97">
-      <c r="CS360" s="4"/>
-    </row>
-    <row r="361" spans="97:97">
-      <c r="CS361" s="4"/>
-    </row>
-    <row r="362" spans="97:97">
-      <c r="CS362" s="4"/>
-    </row>
-    <row r="363" spans="97:97">
-      <c r="CS363" s="4"/>
-    </row>
-    <row r="364" spans="97:97">
-      <c r="CS364" s="4"/>
-    </row>
-    <row r="365" spans="97:97">
-      <c r="CS365" s="4"/>
-    </row>
-    <row r="366" spans="97:97">
-      <c r="CS366" s="4"/>
-    </row>
-    <row r="367" spans="97:97">
-      <c r="CS367" s="4"/>
-    </row>
-    <row r="368" spans="97:97">
-      <c r="CS368" s="4"/>
-    </row>
-    <row r="369" spans="97:97">
-      <c r="CS369" s="4"/>
-    </row>
-    <row r="370" spans="97:97">
-      <c r="CS370" s="4"/>
-    </row>
-    <row r="371" spans="97:97">
-      <c r="CS371" s="4"/>
-    </row>
-    <row r="372" spans="97:97">
-      <c r="CS372" s="4"/>
-    </row>
-    <row r="373" spans="97:97">
-      <c r="CS373" s="4"/>
-    </row>
-    <row r="374" spans="97:97">
-      <c r="CS374" s="4"/>
-    </row>
-    <row r="375" spans="97:97">
-      <c r="CS375" s="4"/>
-    </row>
-    <row r="376" spans="97:97">
-      <c r="CS376" s="4"/>
-    </row>
-    <row r="377" spans="97:97">
-      <c r="CS377" s="4"/>
-    </row>
-    <row r="378" spans="97:97">
-      <c r="CS378" s="4"/>
-    </row>
-    <row r="379" spans="97:97">
-      <c r="CS379" s="4"/>
-    </row>
-    <row r="380" spans="97:97">
-      <c r="CS380" s="4"/>
-    </row>
-    <row r="381" spans="97:97">
-      <c r="CS381" s="4"/>
-    </row>
-    <row r="382" spans="97:97">
-      <c r="CS382" s="4"/>
-    </row>
-    <row r="383" spans="97:97">
-      <c r="CS383" s="4"/>
-    </row>
-    <row r="384" spans="97:97">
-      <c r="CS384" s="4"/>
-    </row>
-    <row r="385" spans="97:97">
-      <c r="CS385" s="4"/>
-    </row>
-    <row r="386" spans="97:97">
-      <c r="CS386" s="4"/>
+    <row r="24" spans="1:96">
+      <c r="CR24" s="4"/>
+    </row>
+    <row r="25" spans="1:96">
+      <c r="CR25" s="4"/>
+    </row>
+    <row r="26" spans="1:96">
+      <c r="CR26" s="4"/>
+    </row>
+    <row r="27" spans="1:96">
+      <c r="CR27" s="4"/>
+    </row>
+    <row r="28" spans="1:96">
+      <c r="CR28" s="4"/>
+    </row>
+    <row r="29" spans="1:96">
+      <c r="CR29" s="4"/>
+    </row>
+    <row r="30" spans="1:96">
+      <c r="CR30" s="4"/>
+    </row>
+    <row r="31" spans="1:96">
+      <c r="CR31" s="4"/>
+    </row>
+    <row r="32" spans="1:96">
+      <c r="CR32" s="4"/>
+    </row>
+    <row r="33" spans="96:96">
+      <c r="CR33" s="4"/>
+    </row>
+    <row r="34" spans="96:96">
+      <c r="CR34" s="4"/>
+    </row>
+    <row r="35" spans="96:96">
+      <c r="CR35" s="4"/>
+    </row>
+    <row r="36" spans="96:96">
+      <c r="CR36" s="4"/>
+    </row>
+    <row r="37" spans="96:96">
+      <c r="CR37" s="4"/>
+    </row>
+    <row r="38" spans="96:96">
+      <c r="CR38" s="4"/>
+    </row>
+    <row r="39" spans="96:96">
+      <c r="CR39" s="4"/>
+    </row>
+    <row r="40" spans="96:96">
+      <c r="CR40" s="4"/>
+    </row>
+    <row r="41" spans="96:96">
+      <c r="CR41" s="4"/>
+    </row>
+    <row r="42" spans="96:96">
+      <c r="CR42" s="4"/>
+    </row>
+    <row r="43" spans="96:96">
+      <c r="CR43" s="4"/>
+    </row>
+    <row r="44" spans="96:96">
+      <c r="CR44" s="4"/>
+    </row>
+    <row r="45" spans="96:96">
+      <c r="CR45" s="4"/>
+    </row>
+    <row r="46" spans="96:96">
+      <c r="CR46" s="4"/>
+    </row>
+    <row r="47" spans="96:96">
+      <c r="CR47" s="4"/>
+    </row>
+    <row r="48" spans="96:96">
+      <c r="CR48" s="4"/>
+    </row>
+    <row r="49" spans="96:96">
+      <c r="CR49" s="4"/>
+    </row>
+    <row r="50" spans="96:96">
+      <c r="CR50" s="4"/>
+    </row>
+    <row r="51" spans="96:96">
+      <c r="CR51" s="4"/>
+    </row>
+    <row r="52" spans="96:96">
+      <c r="CR52" s="4"/>
+    </row>
+    <row r="53" spans="96:96">
+      <c r="CR53" s="4"/>
+    </row>
+    <row r="54" spans="96:96">
+      <c r="CR54" s="4"/>
+    </row>
+    <row r="55" spans="96:96">
+      <c r="CR55" s="4"/>
+    </row>
+    <row r="56" spans="96:96">
+      <c r="CR56" s="4"/>
+    </row>
+    <row r="57" spans="96:96">
+      <c r="CR57" s="4"/>
+    </row>
+    <row r="58" spans="96:96">
+      <c r="CR58" s="4"/>
+    </row>
+    <row r="59" spans="96:96">
+      <c r="CR59" s="4"/>
+    </row>
+    <row r="60" spans="96:96">
+      <c r="CR60" s="4"/>
+    </row>
+    <row r="61" spans="96:96">
+      <c r="CR61" s="4"/>
+    </row>
+    <row r="62" spans="96:96">
+      <c r="CR62" s="4"/>
+    </row>
+    <row r="63" spans="96:96">
+      <c r="CR63" s="4"/>
+    </row>
+    <row r="64" spans="96:96">
+      <c r="CR64" s="4"/>
+    </row>
+    <row r="65" spans="96:96">
+      <c r="CR65" s="4"/>
+    </row>
+    <row r="66" spans="96:96">
+      <c r="CR66" s="4"/>
+    </row>
+    <row r="67" spans="96:96">
+      <c r="CR67" s="4"/>
+    </row>
+    <row r="68" spans="96:96">
+      <c r="CR68" s="4"/>
+    </row>
+    <row r="69" spans="96:96">
+      <c r="CR69" s="4"/>
+    </row>
+    <row r="70" spans="96:96">
+      <c r="CR70" s="4"/>
+    </row>
+    <row r="71" spans="96:96">
+      <c r="CR71" s="4"/>
+    </row>
+    <row r="72" spans="96:96">
+      <c r="CR72" s="4"/>
+    </row>
+    <row r="73" spans="96:96">
+      <c r="CR73" s="4"/>
+    </row>
+    <row r="74" spans="96:96">
+      <c r="CR74" s="4"/>
+    </row>
+    <row r="75" spans="96:96">
+      <c r="CR75" s="4"/>
+    </row>
+    <row r="76" spans="96:96">
+      <c r="CR76" s="4"/>
+    </row>
+    <row r="77" spans="96:96">
+      <c r="CR77" s="4"/>
+    </row>
+    <row r="78" spans="96:96">
+      <c r="CR78" s="4"/>
+    </row>
+    <row r="79" spans="96:96">
+      <c r="CR79" s="4"/>
+    </row>
+    <row r="80" spans="96:96">
+      <c r="CR80" s="4"/>
+    </row>
+    <row r="81" spans="96:96">
+      <c r="CR81" s="4"/>
+    </row>
+    <row r="82" spans="96:96">
+      <c r="CR82" s="4"/>
+    </row>
+    <row r="83" spans="96:96">
+      <c r="CR83" s="4"/>
+    </row>
+    <row r="84" spans="96:96">
+      <c r="CR84" s="4"/>
+    </row>
+    <row r="85" spans="96:96">
+      <c r="CR85" s="4"/>
+    </row>
+    <row r="86" spans="96:96">
+      <c r="CR86" s="4"/>
+    </row>
+    <row r="87" spans="96:96">
+      <c r="CR87" s="4"/>
+    </row>
+    <row r="88" spans="96:96">
+      <c r="CR88" s="4"/>
+    </row>
+    <row r="89" spans="96:96">
+      <c r="CR89" s="4"/>
+    </row>
+    <row r="90" spans="96:96">
+      <c r="CR90" s="4"/>
+    </row>
+    <row r="91" spans="96:96">
+      <c r="CR91" s="4"/>
+    </row>
+    <row r="92" spans="96:96">
+      <c r="CR92" s="4"/>
+    </row>
+    <row r="93" spans="96:96">
+      <c r="CR93" s="4"/>
+    </row>
+    <row r="94" spans="96:96">
+      <c r="CR94" s="4"/>
+    </row>
+    <row r="95" spans="96:96">
+      <c r="CR95" s="4"/>
+    </row>
+    <row r="96" spans="96:96">
+      <c r="CR96" s="4"/>
+    </row>
+    <row r="97" spans="96:96">
+      <c r="CR97" s="4"/>
+    </row>
+    <row r="98" spans="96:96">
+      <c r="CR98" s="4"/>
+    </row>
+    <row r="99" spans="96:96">
+      <c r="CR99" s="4"/>
+    </row>
+    <row r="100" spans="96:96">
+      <c r="CR100" s="4"/>
+    </row>
+    <row r="101" spans="96:96">
+      <c r="CR101" s="4"/>
+    </row>
+    <row r="102" spans="96:96">
+      <c r="CR102" s="4"/>
+    </row>
+    <row r="103" spans="96:96">
+      <c r="CR103" s="4"/>
+    </row>
+    <row r="104" spans="96:96">
+      <c r="CR104" s="4"/>
+    </row>
+    <row r="105" spans="96:96">
+      <c r="CR105" s="4"/>
+    </row>
+    <row r="106" spans="96:96">
+      <c r="CR106" s="4"/>
+    </row>
+    <row r="107" spans="96:96">
+      <c r="CR107" s="4"/>
+    </row>
+    <row r="108" spans="96:96">
+      <c r="CR108" s="4"/>
+    </row>
+    <row r="109" spans="96:96">
+      <c r="CR109" s="4"/>
+    </row>
+    <row r="110" spans="96:96">
+      <c r="CR110" s="4"/>
+    </row>
+    <row r="111" spans="96:96">
+      <c r="CR111" s="4"/>
+    </row>
+    <row r="112" spans="96:96">
+      <c r="CR112" s="4"/>
+    </row>
+    <row r="113" spans="96:96">
+      <c r="CR113" s="4"/>
+    </row>
+    <row r="114" spans="96:96">
+      <c r="CR114" s="4"/>
+    </row>
+    <row r="115" spans="96:96">
+      <c r="CR115" s="4"/>
+    </row>
+    <row r="116" spans="96:96">
+      <c r="CR116" s="4"/>
+    </row>
+    <row r="117" spans="96:96">
+      <c r="CR117" s="4"/>
+    </row>
+    <row r="118" spans="96:96">
+      <c r="CR118" s="4"/>
+    </row>
+    <row r="119" spans="96:96">
+      <c r="CR119" s="4"/>
+    </row>
+    <row r="120" spans="96:96">
+      <c r="CR120" s="4"/>
+    </row>
+    <row r="121" spans="96:96">
+      <c r="CR121" s="4"/>
+    </row>
+    <row r="122" spans="96:96">
+      <c r="CR122" s="4"/>
+    </row>
+    <row r="123" spans="96:96">
+      <c r="CR123" s="4"/>
+    </row>
+    <row r="124" spans="96:96">
+      <c r="CR124" s="4"/>
+    </row>
+    <row r="125" spans="96:96">
+      <c r="CR125" s="4"/>
+    </row>
+    <row r="126" spans="96:96">
+      <c r="CR126" s="4"/>
+    </row>
+    <row r="127" spans="96:96">
+      <c r="CR127" s="4"/>
+    </row>
+    <row r="128" spans="96:96">
+      <c r="CR128" s="4"/>
+    </row>
+    <row r="129" spans="96:96">
+      <c r="CR129" s="4"/>
+    </row>
+    <row r="130" spans="96:96">
+      <c r="CR130" s="4"/>
+    </row>
+    <row r="131" spans="96:96">
+      <c r="CR131" s="4"/>
+    </row>
+    <row r="132" spans="96:96">
+      <c r="CR132" s="4"/>
+    </row>
+    <row r="133" spans="96:96">
+      <c r="CR133" s="4"/>
+    </row>
+    <row r="134" spans="96:96">
+      <c r="CR134" s="4"/>
+    </row>
+    <row r="135" spans="96:96">
+      <c r="CR135" s="4"/>
+    </row>
+    <row r="136" spans="96:96">
+      <c r="CR136" s="4"/>
+    </row>
+    <row r="137" spans="96:96">
+      <c r="CR137" s="4"/>
+    </row>
+    <row r="138" spans="96:96">
+      <c r="CR138" s="4"/>
+    </row>
+    <row r="139" spans="96:96">
+      <c r="CR139" s="4"/>
+    </row>
+    <row r="140" spans="96:96">
+      <c r="CR140" s="4"/>
+    </row>
+    <row r="141" spans="96:96">
+      <c r="CR141" s="4"/>
+    </row>
+    <row r="142" spans="96:96">
+      <c r="CR142" s="4"/>
+    </row>
+    <row r="143" spans="96:96">
+      <c r="CR143" s="4"/>
+    </row>
+    <row r="144" spans="96:96">
+      <c r="CR144" s="4"/>
+    </row>
+    <row r="145" spans="96:96">
+      <c r="CR145" s="4"/>
+    </row>
+    <row r="146" spans="96:96">
+      <c r="CR146" s="4"/>
+    </row>
+    <row r="147" spans="96:96">
+      <c r="CR147" s="4"/>
+    </row>
+    <row r="148" spans="96:96">
+      <c r="CR148" s="4"/>
+    </row>
+    <row r="149" spans="96:96">
+      <c r="CR149" s="4"/>
+    </row>
+    <row r="150" spans="96:96">
+      <c r="CR150" s="4"/>
+    </row>
+    <row r="151" spans="96:96">
+      <c r="CR151" s="4"/>
+    </row>
+    <row r="152" spans="96:96">
+      <c r="CR152" s="4"/>
+    </row>
+    <row r="153" spans="96:96">
+      <c r="CR153" s="4"/>
+    </row>
+    <row r="154" spans="96:96">
+      <c r="CR154" s="4"/>
+    </row>
+    <row r="155" spans="96:96">
+      <c r="CR155" s="4"/>
+    </row>
+    <row r="156" spans="96:96">
+      <c r="CR156" s="4"/>
+    </row>
+    <row r="157" spans="96:96">
+      <c r="CR157" s="4"/>
+    </row>
+    <row r="158" spans="96:96">
+      <c r="CR158" s="4"/>
+    </row>
+    <row r="159" spans="96:96">
+      <c r="CR159" s="4"/>
+    </row>
+    <row r="160" spans="96:96">
+      <c r="CR160" s="4"/>
+    </row>
+    <row r="161" spans="96:96">
+      <c r="CR161" s="4"/>
+    </row>
+    <row r="162" spans="96:96">
+      <c r="CR162" s="4"/>
+    </row>
+    <row r="163" spans="96:96">
+      <c r="CR163" s="4"/>
+    </row>
+    <row r="164" spans="96:96">
+      <c r="CR164" s="4"/>
+    </row>
+    <row r="165" spans="96:96">
+      <c r="CR165" s="4"/>
+    </row>
+    <row r="166" spans="96:96">
+      <c r="CR166" s="4"/>
+    </row>
+    <row r="167" spans="96:96">
+      <c r="CR167" s="4"/>
+    </row>
+    <row r="168" spans="96:96">
+      <c r="CR168" s="4"/>
+    </row>
+    <row r="169" spans="96:96">
+      <c r="CR169" s="4"/>
+    </row>
+    <row r="170" spans="96:96">
+      <c r="CR170" s="4"/>
+    </row>
+    <row r="171" spans="96:96">
+      <c r="CR171" s="4"/>
+    </row>
+    <row r="172" spans="96:96">
+      <c r="CR172" s="4"/>
+    </row>
+    <row r="173" spans="96:96">
+      <c r="CR173" s="4"/>
+    </row>
+    <row r="174" spans="96:96">
+      <c r="CR174" s="4"/>
+    </row>
+    <row r="175" spans="96:96">
+      <c r="CR175" s="4"/>
+    </row>
+    <row r="176" spans="96:96">
+      <c r="CR176" s="4"/>
+    </row>
+    <row r="177" spans="96:96">
+      <c r="CR177" s="4"/>
+    </row>
+    <row r="178" spans="96:96">
+      <c r="CR178" s="4"/>
+    </row>
+    <row r="179" spans="96:96">
+      <c r="CR179" s="4"/>
+    </row>
+    <row r="180" spans="96:96">
+      <c r="CR180" s="4"/>
+    </row>
+    <row r="181" spans="96:96">
+      <c r="CR181" s="4"/>
+    </row>
+    <row r="182" spans="96:96">
+      <c r="CR182" s="4"/>
+    </row>
+    <row r="183" spans="96:96">
+      <c r="CR183" s="4"/>
+    </row>
+    <row r="184" spans="96:96">
+      <c r="CR184" s="4"/>
+    </row>
+    <row r="185" spans="96:96">
+      <c r="CR185" s="4"/>
+    </row>
+    <row r="186" spans="96:96">
+      <c r="CR186" s="4"/>
+    </row>
+    <row r="187" spans="96:96">
+      <c r="CR187" s="4"/>
+    </row>
+    <row r="188" spans="96:96">
+      <c r="CR188" s="4"/>
+    </row>
+    <row r="189" spans="96:96">
+      <c r="CR189" s="4"/>
+    </row>
+    <row r="190" spans="96:96">
+      <c r="CR190" s="4"/>
+    </row>
+    <row r="191" spans="96:96">
+      <c r="CR191" s="4"/>
+    </row>
+    <row r="192" spans="96:96">
+      <c r="CR192" s="4"/>
+    </row>
+    <row r="193" spans="96:96">
+      <c r="CR193" s="4"/>
+    </row>
+    <row r="194" spans="96:96">
+      <c r="CR194" s="4"/>
+    </row>
+    <row r="195" spans="96:96">
+      <c r="CR195" s="4"/>
+    </row>
+    <row r="196" spans="96:96">
+      <c r="CR196" s="4"/>
+    </row>
+    <row r="197" spans="96:96">
+      <c r="CR197" s="4"/>
+    </row>
+    <row r="198" spans="96:96">
+      <c r="CR198" s="4"/>
+    </row>
+    <row r="199" spans="96:96">
+      <c r="CR199" s="4"/>
+    </row>
+    <row r="200" spans="96:96">
+      <c r="CR200" s="4"/>
+    </row>
+    <row r="201" spans="96:96">
+      <c r="CR201" s="4"/>
+    </row>
+    <row r="202" spans="96:96">
+      <c r="CR202" s="4"/>
+    </row>
+    <row r="203" spans="96:96">
+      <c r="CR203" s="4"/>
+    </row>
+    <row r="204" spans="96:96">
+      <c r="CR204" s="4"/>
+    </row>
+    <row r="205" spans="96:96">
+      <c r="CR205" s="4"/>
+    </row>
+    <row r="206" spans="96:96">
+      <c r="CR206" s="4"/>
+    </row>
+    <row r="207" spans="96:96">
+      <c r="CR207" s="4"/>
+    </row>
+    <row r="208" spans="96:96">
+      <c r="CR208" s="4"/>
+    </row>
+    <row r="209" spans="96:96">
+      <c r="CR209" s="4"/>
+    </row>
+    <row r="210" spans="96:96">
+      <c r="CR210" s="4"/>
+    </row>
+    <row r="211" spans="96:96">
+      <c r="CR211" s="4"/>
+    </row>
+    <row r="212" spans="96:96">
+      <c r="CR212" s="4"/>
+    </row>
+    <row r="213" spans="96:96">
+      <c r="CR213" s="4"/>
+    </row>
+    <row r="214" spans="96:96">
+      <c r="CR214" s="4"/>
+    </row>
+    <row r="215" spans="96:96">
+      <c r="CR215" s="4"/>
+    </row>
+    <row r="216" spans="96:96">
+      <c r="CR216" s="4"/>
+    </row>
+    <row r="217" spans="96:96">
+      <c r="CR217" s="4"/>
+    </row>
+    <row r="218" spans="96:96">
+      <c r="CR218" s="4"/>
+    </row>
+    <row r="219" spans="96:96">
+      <c r="CR219" s="4"/>
+    </row>
+    <row r="220" spans="96:96">
+      <c r="CR220" s="4"/>
+    </row>
+    <row r="221" spans="96:96">
+      <c r="CR221" s="4"/>
+    </row>
+    <row r="222" spans="96:96">
+      <c r="CR222" s="4"/>
+    </row>
+    <row r="223" spans="96:96">
+      <c r="CR223" s="4"/>
+    </row>
+    <row r="224" spans="96:96">
+      <c r="CR224" s="4"/>
+    </row>
+    <row r="225" spans="96:96">
+      <c r="CR225" s="4"/>
+    </row>
+    <row r="226" spans="96:96">
+      <c r="CR226" s="4"/>
+    </row>
+    <row r="227" spans="96:96">
+      <c r="CR227" s="4"/>
+    </row>
+    <row r="228" spans="96:96">
+      <c r="CR228" s="4"/>
+    </row>
+    <row r="229" spans="96:96">
+      <c r="CR229" s="4"/>
+    </row>
+    <row r="230" spans="96:96">
+      <c r="CR230" s="4"/>
+    </row>
+    <row r="231" spans="96:96">
+      <c r="CR231" s="4"/>
+    </row>
+    <row r="232" spans="96:96">
+      <c r="CR232" s="4"/>
+    </row>
+    <row r="233" spans="96:96">
+      <c r="CR233" s="4"/>
+    </row>
+    <row r="234" spans="96:96">
+      <c r="CR234" s="4"/>
+    </row>
+    <row r="235" spans="96:96">
+      <c r="CR235" s="4"/>
+    </row>
+    <row r="236" spans="96:96">
+      <c r="CR236" s="4"/>
+    </row>
+    <row r="237" spans="96:96">
+      <c r="CR237" s="4"/>
+    </row>
+    <row r="238" spans="96:96">
+      <c r="CR238" s="4"/>
+    </row>
+    <row r="239" spans="96:96">
+      <c r="CR239" s="4"/>
+    </row>
+    <row r="240" spans="96:96">
+      <c r="CR240" s="4"/>
+    </row>
+    <row r="241" spans="96:96">
+      <c r="CR241" s="4"/>
+    </row>
+    <row r="242" spans="96:96">
+      <c r="CR242" s="4"/>
+    </row>
+    <row r="243" spans="96:96">
+      <c r="CR243" s="4"/>
+    </row>
+    <row r="244" spans="96:96">
+      <c r="CR244" s="4"/>
+    </row>
+    <row r="245" spans="96:96">
+      <c r="CR245" s="4"/>
+    </row>
+    <row r="246" spans="96:96">
+      <c r="CR246" s="4"/>
+    </row>
+    <row r="247" spans="96:96">
+      <c r="CR247" s="4"/>
+    </row>
+    <row r="248" spans="96:96">
+      <c r="CR248" s="4"/>
+    </row>
+    <row r="249" spans="96:96">
+      <c r="CR249" s="4"/>
+    </row>
+    <row r="250" spans="96:96">
+      <c r="CR250" s="4"/>
+    </row>
+    <row r="251" spans="96:96">
+      <c r="CR251" s="4"/>
+    </row>
+    <row r="252" spans="96:96">
+      <c r="CR252" s="4"/>
+    </row>
+    <row r="253" spans="96:96">
+      <c r="CR253" s="4"/>
+    </row>
+    <row r="254" spans="96:96">
+      <c r="CR254" s="4"/>
+    </row>
+    <row r="255" spans="96:96">
+      <c r="CR255" s="4"/>
+    </row>
+    <row r="256" spans="96:96">
+      <c r="CR256" s="4"/>
+    </row>
+    <row r="257" spans="96:96">
+      <c r="CR257" s="4"/>
+    </row>
+    <row r="258" spans="96:96">
+      <c r="CR258" s="4"/>
+    </row>
+    <row r="259" spans="96:96">
+      <c r="CR259" s="4"/>
+    </row>
+    <row r="260" spans="96:96">
+      <c r="CR260" s="4"/>
+    </row>
+    <row r="261" spans="96:96">
+      <c r="CR261" s="4"/>
+    </row>
+    <row r="262" spans="96:96">
+      <c r="CR262" s="4"/>
+    </row>
+    <row r="263" spans="96:96">
+      <c r="CR263" s="4"/>
+    </row>
+    <row r="264" spans="96:96">
+      <c r="CR264" s="4"/>
+    </row>
+    <row r="265" spans="96:96">
+      <c r="CR265" s="4"/>
+    </row>
+    <row r="266" spans="96:96">
+      <c r="CR266" s="4"/>
+    </row>
+    <row r="267" spans="96:96">
+      <c r="CR267" s="4"/>
+    </row>
+    <row r="268" spans="96:96">
+      <c r="CR268" s="4"/>
+    </row>
+    <row r="269" spans="96:96">
+      <c r="CR269" s="4"/>
+    </row>
+    <row r="270" spans="96:96">
+      <c r="CR270" s="4"/>
+    </row>
+    <row r="271" spans="96:96">
+      <c r="CR271" s="4"/>
+    </row>
+    <row r="272" spans="96:96">
+      <c r="CR272" s="4"/>
+    </row>
+    <row r="273" spans="96:96">
+      <c r="CR273" s="4"/>
+    </row>
+    <row r="274" spans="96:96">
+      <c r="CR274" s="4"/>
+    </row>
+    <row r="275" spans="96:96">
+      <c r="CR275" s="4"/>
+    </row>
+    <row r="276" spans="96:96">
+      <c r="CR276" s="4"/>
+    </row>
+    <row r="277" spans="96:96">
+      <c r="CR277" s="4"/>
+    </row>
+    <row r="278" spans="96:96">
+      <c r="CR278" s="4"/>
+    </row>
+    <row r="279" spans="96:96">
+      <c r="CR279" s="4"/>
+    </row>
+    <row r="280" spans="96:96">
+      <c r="CR280" s="4"/>
+    </row>
+    <row r="281" spans="96:96">
+      <c r="CR281" s="4"/>
+    </row>
+    <row r="282" spans="96:96">
+      <c r="CR282" s="4"/>
+    </row>
+    <row r="283" spans="96:96">
+      <c r="CR283" s="4"/>
+    </row>
+    <row r="284" spans="96:96">
+      <c r="CR284" s="4"/>
+    </row>
+    <row r="285" spans="96:96">
+      <c r="CR285" s="4"/>
+    </row>
+    <row r="286" spans="96:96">
+      <c r="CR286" s="4"/>
+    </row>
+    <row r="287" spans="96:96">
+      <c r="CR287" s="4"/>
+    </row>
+    <row r="288" spans="96:96">
+      <c r="CR288" s="4"/>
+    </row>
+    <row r="289" spans="96:96">
+      <c r="CR289" s="4"/>
+    </row>
+    <row r="290" spans="96:96">
+      <c r="CR290" s="4"/>
+    </row>
+    <row r="291" spans="96:96">
+      <c r="CR291" s="4"/>
+    </row>
+    <row r="292" spans="96:96">
+      <c r="CR292" s="4"/>
+    </row>
+    <row r="293" spans="96:96">
+      <c r="CR293" s="4"/>
+    </row>
+    <row r="294" spans="96:96">
+      <c r="CR294" s="4"/>
+    </row>
+    <row r="295" spans="96:96">
+      <c r="CR295" s="4"/>
+    </row>
+    <row r="296" spans="96:96">
+      <c r="CR296" s="4"/>
+    </row>
+    <row r="297" spans="96:96">
+      <c r="CR297" s="4"/>
+    </row>
+    <row r="298" spans="96:96">
+      <c r="CR298" s="4"/>
+    </row>
+    <row r="299" spans="96:96">
+      <c r="CR299" s="4"/>
+    </row>
+    <row r="300" spans="96:96">
+      <c r="CR300" s="4"/>
+    </row>
+    <row r="301" spans="96:96">
+      <c r="CR301" s="4"/>
+    </row>
+    <row r="302" spans="96:96">
+      <c r="CR302" s="4"/>
+    </row>
+    <row r="303" spans="96:96">
+      <c r="CR303" s="4"/>
+    </row>
+    <row r="304" spans="96:96">
+      <c r="CR304" s="4"/>
+    </row>
+    <row r="305" spans="96:96">
+      <c r="CR305" s="4"/>
+    </row>
+    <row r="306" spans="96:96">
+      <c r="CR306" s="4"/>
+    </row>
+    <row r="307" spans="96:96">
+      <c r="CR307" s="4"/>
+    </row>
+    <row r="308" spans="96:96">
+      <c r="CR308" s="4"/>
+    </row>
+    <row r="309" spans="96:96">
+      <c r="CR309" s="4"/>
+    </row>
+    <row r="310" spans="96:96">
+      <c r="CR310" s="4"/>
+    </row>
+    <row r="311" spans="96:96">
+      <c r="CR311" s="4"/>
+    </row>
+    <row r="312" spans="96:96">
+      <c r="CR312" s="4"/>
+    </row>
+    <row r="313" spans="96:96">
+      <c r="CR313" s="4"/>
+    </row>
+    <row r="314" spans="96:96">
+      <c r="CR314" s="4"/>
+    </row>
+    <row r="315" spans="96:96">
+      <c r="CR315" s="4"/>
+    </row>
+    <row r="316" spans="96:96">
+      <c r="CR316" s="4"/>
+    </row>
+    <row r="317" spans="96:96">
+      <c r="CR317" s="4"/>
+    </row>
+    <row r="318" spans="96:96">
+      <c r="CR318" s="4"/>
+    </row>
+    <row r="319" spans="96:96">
+      <c r="CR319" s="4"/>
+    </row>
+    <row r="320" spans="96:96">
+      <c r="CR320" s="4"/>
+    </row>
+    <row r="321" spans="96:96">
+      <c r="CR321" s="4"/>
+    </row>
+    <row r="322" spans="96:96">
+      <c r="CR322" s="4"/>
+    </row>
+    <row r="323" spans="96:96">
+      <c r="CR323" s="4"/>
+    </row>
+    <row r="324" spans="96:96">
+      <c r="CR324" s="4"/>
+    </row>
+    <row r="325" spans="96:96">
+      <c r="CR325" s="4"/>
+    </row>
+    <row r="326" spans="96:96">
+      <c r="CR326" s="4"/>
+    </row>
+    <row r="327" spans="96:96">
+      <c r="CR327" s="4"/>
+    </row>
+    <row r="328" spans="96:96">
+      <c r="CR328" s="4"/>
+    </row>
+    <row r="329" spans="96:96">
+      <c r="CR329" s="4"/>
+    </row>
+    <row r="330" spans="96:96">
+      <c r="CR330" s="4"/>
+    </row>
+    <row r="331" spans="96:96">
+      <c r="CR331" s="4"/>
+    </row>
+    <row r="332" spans="96:96">
+      <c r="CR332" s="4"/>
+    </row>
+    <row r="333" spans="96:96">
+      <c r="CR333" s="4"/>
+    </row>
+    <row r="334" spans="96:96">
+      <c r="CR334" s="4"/>
+    </row>
+    <row r="335" spans="96:96">
+      <c r="CR335" s="4"/>
+    </row>
+    <row r="336" spans="96:96">
+      <c r="CR336" s="4"/>
+    </row>
+    <row r="337" spans="96:96">
+      <c r="CR337" s="4"/>
+    </row>
+    <row r="338" spans="96:96">
+      <c r="CR338" s="4"/>
+    </row>
+    <row r="339" spans="96:96">
+      <c r="CR339" s="4"/>
+    </row>
+    <row r="340" spans="96:96">
+      <c r="CR340" s="4"/>
+    </row>
+    <row r="341" spans="96:96">
+      <c r="CR341" s="4"/>
+    </row>
+    <row r="342" spans="96:96">
+      <c r="CR342" s="4"/>
+    </row>
+    <row r="343" spans="96:96">
+      <c r="CR343" s="4"/>
+    </row>
+    <row r="344" spans="96:96">
+      <c r="CR344" s="4"/>
+    </row>
+    <row r="345" spans="96:96">
+      <c r="CR345" s="4"/>
+    </row>
+    <row r="346" spans="96:96">
+      <c r="CR346" s="4"/>
+    </row>
+    <row r="347" spans="96:96">
+      <c r="CR347" s="4"/>
+    </row>
+    <row r="348" spans="96:96">
+      <c r="CR348" s="4"/>
+    </row>
+    <row r="349" spans="96:96">
+      <c r="CR349" s="4"/>
+    </row>
+    <row r="350" spans="96:96">
+      <c r="CR350" s="4"/>
+    </row>
+    <row r="351" spans="96:96">
+      <c r="CR351" s="4"/>
+    </row>
+    <row r="352" spans="96:96">
+      <c r="CR352" s="4"/>
+    </row>
+    <row r="353" spans="96:96">
+      <c r="CR353" s="4"/>
+    </row>
+    <row r="354" spans="96:96">
+      <c r="CR354" s="4"/>
+    </row>
+    <row r="355" spans="96:96">
+      <c r="CR355" s="4"/>
+    </row>
+    <row r="356" spans="96:96">
+      <c r="CR356" s="4"/>
+    </row>
+    <row r="357" spans="96:96">
+      <c r="CR357" s="4"/>
+    </row>
+    <row r="358" spans="96:96">
+      <c r="CR358" s="4"/>
+    </row>
+    <row r="359" spans="96:96">
+      <c r="CR359" s="4"/>
+    </row>
+    <row r="360" spans="96:96">
+      <c r="CR360" s="4"/>
+    </row>
+    <row r="361" spans="96:96">
+      <c r="CR361" s="4"/>
+    </row>
+    <row r="362" spans="96:96">
+      <c r="CR362" s="4"/>
+    </row>
+    <row r="363" spans="96:96">
+      <c r="CR363" s="4"/>
+    </row>
+    <row r="364" spans="96:96">
+      <c r="CR364" s="4"/>
+    </row>
+    <row r="365" spans="96:96">
+      <c r="CR365" s="4"/>
+    </row>
+    <row r="366" spans="96:96">
+      <c r="CR366" s="4"/>
+    </row>
+    <row r="367" spans="96:96">
+      <c r="CR367" s="4"/>
+    </row>
+    <row r="368" spans="96:96">
+      <c r="CR368" s="4"/>
+    </row>
+    <row r="369" spans="96:96">
+      <c r="CR369" s="4"/>
+    </row>
+    <row r="370" spans="96:96">
+      <c r="CR370" s="4"/>
+    </row>
+    <row r="371" spans="96:96">
+      <c r="CR371" s="4"/>
+    </row>
+    <row r="372" spans="96:96">
+      <c r="CR372" s="4"/>
+    </row>
+    <row r="373" spans="96:96">
+      <c r="CR373" s="4"/>
+    </row>
+    <row r="374" spans="96:96">
+      <c r="CR374" s="4"/>
+    </row>
+    <row r="375" spans="96:96">
+      <c r="CR375" s="4"/>
+    </row>
+    <row r="376" spans="96:96">
+      <c r="CR376" s="4"/>
+    </row>
+    <row r="377" spans="96:96">
+      <c r="CR377" s="4"/>
+    </row>
+    <row r="378" spans="96:96">
+      <c r="CR378" s="4"/>
+    </row>
+    <row r="379" spans="96:96">
+      <c r="CR379" s="4"/>
+    </row>
+    <row r="380" spans="96:96">
+      <c r="CR380" s="4"/>
+    </row>
+    <row r="381" spans="96:96">
+      <c r="CR381" s="4"/>
+    </row>
+    <row r="382" spans="96:96">
+      <c r="CR382" s="4"/>
+    </row>
+    <row r="383" spans="96:96">
+      <c r="CR383" s="4"/>
+    </row>
+    <row r="384" spans="96:96">
+      <c r="CR384" s="4"/>
+    </row>
+    <row r="385" spans="96:96">
+      <c r="CR385" s="4"/>
+    </row>
+    <row r="386" spans="96:96">
+      <c r="CR386" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3409,7 +3401,7 @@
           <x14:formula1>
             <xm:f>validation!$J$2:$J$14</xm:f>
           </x14:formula1>
-          <xm:sqref>BW147:BW1048576 CC2:CC1048576 CI2:CI1048576</xm:sqref>
+          <xm:sqref>BV147:BV1048576 CB2:CB1048576 CH2:CH1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -3421,19 +3413,19 @@
           <x14:formula1>
             <xm:f>validation!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>CP51:CP1048576 S5:S380 R2:S4 L2:M1048576 BN2:BN385 W2:W385 G2:G374 BP2:BP1048576 R5:R266</xm:sqref>
+          <xm:sqref>CO51:CO1048576 L2:M1048576 BM2:BM385 V2:V385 G2:G374 BO2:BO1048576 R2:R380</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>validation!$G$2:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>Y384:Y1048576</xm:sqref>
+          <xm:sqref>X384:X1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>validation!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>CH2:CH1048576 CB2:CB1048576</xm:sqref>
+          <xm:sqref>CG2:CG1048576 CA2:CA1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
@@ -3445,7 +3437,7 @@
           <x14:formula1>
             <xm:f>validation!$K$2:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>BY2:CA1048576 CE2:CG1048576 CK2:CM1048576</xm:sqref>
+          <xm:sqref>BX2:BZ1048576 CD2:CF1048576 CJ2:CL1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
@@ -3463,13 +3455,13 @@
           <x14:formula1>
             <xm:f>validation!$H$2:$H$20</xm:f>
           </x14:formula1>
-          <xm:sqref>BA2:BA1048576 AA2:AA507 AN2:AN507</xm:sqref>
+          <xm:sqref>AZ2:AZ1048576 Z2:Z507 AM2:AM507</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{66B143F6-674E-F24D-AC17-D3B9F43B9156}">
           <x14:formula1>
             <xm:f>validation!$J$2:$J$15</xm:f>
           </x14:formula1>
-          <xm:sqref>BW2:BW146</xm:sqref>
+          <xm:sqref>BV2:BV146</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ADD35E30-6BB4-5049-BCED-AA1C79EA5464}">
           <x14:formula1>
@@ -3481,7 +3473,7 @@
           <x14:formula1>
             <xm:f>validation!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>CT2:CT302</xm:sqref>
+          <xm:sqref>CS2:CS302</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3F6A4444-35F1-6448-88BC-C3A1752C8F76}">
           <x14:formula1>
@@ -3499,13 +3491,13 @@
           <x14:formula1>
             <xm:f>validation!$G$2:$G$9</xm:f>
           </x14:formula1>
-          <xm:sqref>Y2:Y383</xm:sqref>
+          <xm:sqref>X2:X383</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EC4E7F5A-47BD-D149-9FC4-9E6ACF2F243A}">
           <x14:formula1>
             <xm:f>validation!$I$2:$I$40</xm:f>
           </x14:formula1>
-          <xm:sqref>BB2:BB1048576 AB2:AB507 AO2:AO507</xm:sqref>
+          <xm:sqref>BA2:BA1048576 AA2:AA507 AN2:AN507</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3554,7 +3546,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>66</v>
@@ -3573,7 +3565,7 @@
         <v>98</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -3591,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -3608,25 +3600,25 @@
         <v>97</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>67</v>
@@ -3649,7 +3641,7 @@
         <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>35</v>
@@ -3658,7 +3650,7 @@
         <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
         <v>111</v>
@@ -3681,7 +3673,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>36</v>
@@ -3707,7 +3699,7 @@
         <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>37</v>
@@ -3724,13 +3716,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>38</v>
@@ -3747,13 +3739,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>106</v>
@@ -3770,10 +3762,10 @@
         <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
@@ -3787,7 +3779,7 @@
         <v>102</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H10" t="s">
         <v>49</v>
@@ -3879,18 +3871,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -3898,7 +3890,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -3906,29 +3898,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3948,24 +3940,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
         <v>197</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>198</v>
-      </c>
-      <c r="C1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51">
       <c r="A2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
         <v>200</v>
-      </c>
-      <c r="C2" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated indicators to list
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1B9BB4-1BB8-3E4F-8082-F157F06D361A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406BDBDC-9D36-DF4F-AFA1-E6AC47B99308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="208">
   <si>
     <t>strategy_name</t>
   </si>
@@ -455,120 +455,6 @@
     <t>Both</t>
   </si>
   <si>
-    <t>first_indicator</t>
-  </si>
-  <si>
-    <t>first_indicator_param_a</t>
-  </si>
-  <si>
-    <t>first_indicator_param_b</t>
-  </si>
-  <si>
-    <t>first_indicator_param_c</t>
-  </si>
-  <si>
-    <t>first_indicator_param_d</t>
-  </si>
-  <si>
-    <t>first_indicator_param_e</t>
-  </si>
-  <si>
-    <t>first_indicator_param_f</t>
-  </si>
-  <si>
-    <t>first_indicator_param_g</t>
-  </si>
-  <si>
-    <t>first_indicator_param_h</t>
-  </si>
-  <si>
-    <t>first_indicator_param_i</t>
-  </si>
-  <si>
-    <t>first_indicator_param_j</t>
-  </si>
-  <si>
-    <t>first_indicator_param_k</t>
-  </si>
-  <si>
-    <t>second_indicator</t>
-  </si>
-  <si>
-    <t>second_indicator_use</t>
-  </si>
-  <si>
-    <t>second_indicator_param_a</t>
-  </si>
-  <si>
-    <t>second_indicator_param_b</t>
-  </si>
-  <si>
-    <t>second_indicator_param_c</t>
-  </si>
-  <si>
-    <t>second_indicator_param_d</t>
-  </si>
-  <si>
-    <t>second_indicator_param_e</t>
-  </si>
-  <si>
-    <t>second_indicator_param_f</t>
-  </si>
-  <si>
-    <t>second_indicator_param_g</t>
-  </si>
-  <si>
-    <t>second_indicator_param_h</t>
-  </si>
-  <si>
-    <t>second_indicator_param_i</t>
-  </si>
-  <si>
-    <t>second_indicator_param_j</t>
-  </si>
-  <si>
-    <t>second_indicator_param_k</t>
-  </si>
-  <si>
-    <t>third_indicator</t>
-  </si>
-  <si>
-    <t>third_indicator_use</t>
-  </si>
-  <si>
-    <t>third_indicator_param_a</t>
-  </si>
-  <si>
-    <t>third_indicator_param_b</t>
-  </si>
-  <si>
-    <t>third_indicator_param_c</t>
-  </si>
-  <si>
-    <t>third_indicator_param_d</t>
-  </si>
-  <si>
-    <t>third_indicator_param_e</t>
-  </si>
-  <si>
-    <t>third_indicator_param_f</t>
-  </si>
-  <si>
-    <t>third_indicator_param_g</t>
-  </si>
-  <si>
-    <t>third_indicator_param_h</t>
-  </si>
-  <si>
-    <t>third_indicator_param_i</t>
-  </si>
-  <si>
-    <t>third_indicator_param_j</t>
-  </si>
-  <si>
-    <t>third_indicator_param_k</t>
-  </si>
-  <si>
     <t>fast_trail_ATR_start_multiplier</t>
   </si>
   <si>
@@ -657,6 +543,123 @@
   </si>
   <si>
     <t>EURGBP;USDJPY</t>
+  </si>
+  <si>
+    <t>indicator_1</t>
+  </si>
+  <si>
+    <t>indicator_1_use</t>
+  </si>
+  <si>
+    <t>indicator_1_param_a</t>
+  </si>
+  <si>
+    <t>indicator_1_param_b</t>
+  </si>
+  <si>
+    <t>indicator_1_param_c</t>
+  </si>
+  <si>
+    <t>indicator_1_param_d</t>
+  </si>
+  <si>
+    <t>indicator_1_param_e</t>
+  </si>
+  <si>
+    <t>indicator_1_param_f</t>
+  </si>
+  <si>
+    <t>indicator_1_param_g</t>
+  </si>
+  <si>
+    <t>indicator_1_param_h</t>
+  </si>
+  <si>
+    <t>indicator_1_param_i</t>
+  </si>
+  <si>
+    <t>indicator_1_param_j</t>
+  </si>
+  <si>
+    <t>indicator_1_param_k</t>
+  </si>
+  <si>
+    <t>indicator_2</t>
+  </si>
+  <si>
+    <t>indicator_2_use</t>
+  </si>
+  <si>
+    <t>indicator_2_param_a</t>
+  </si>
+  <si>
+    <t>indicator_2_param_b</t>
+  </si>
+  <si>
+    <t>indicator_2_param_c</t>
+  </si>
+  <si>
+    <t>indicator_2_param_d</t>
+  </si>
+  <si>
+    <t>indicator_2_param_e</t>
+  </si>
+  <si>
+    <t>indicator_2_param_f</t>
+  </si>
+  <si>
+    <t>indicator_2_param_g</t>
+  </si>
+  <si>
+    <t>indicator_2_param_h</t>
+  </si>
+  <si>
+    <t>indicator_2_param_i</t>
+  </si>
+  <si>
+    <t>indicator_2_param_j</t>
+  </si>
+  <si>
+    <t>indicator_2_param_k</t>
+  </si>
+  <si>
+    <t>indicator_3</t>
+  </si>
+  <si>
+    <t>indicator_3_use</t>
+  </si>
+  <si>
+    <t>indicator_3_param_a</t>
+  </si>
+  <si>
+    <t>indicator_3_param_b</t>
+  </si>
+  <si>
+    <t>indicator_3_param_c</t>
+  </si>
+  <si>
+    <t>indicator_3_param_d</t>
+  </si>
+  <si>
+    <t>indicator_3_param_e</t>
+  </si>
+  <si>
+    <t>indicator_3_param_f</t>
+  </si>
+  <si>
+    <t>indicator_3_param_g</t>
+  </si>
+  <si>
+    <t>indicator_3_param_h</t>
+  </si>
+  <si>
+    <t>indicator_3_param_i</t>
+  </si>
+  <si>
+    <t>indicator_3_param_j</t>
+  </si>
+  <si>
+    <t>indicator_3_param_k</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1529,10 @@
   <dimension ref="A1:CS386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CP2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AX2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CP10" sqref="CP10"/>
+      <selection pane="bottomRight" activeCell="BA11" sqref="BA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -1590,7 +1593,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1629,13 +1632,13 @@
         <v>128</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>130</v>
@@ -1647,121 +1650,121 @@
         <v>40</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>158</v>
+        <v>189</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="BM1" s="1" t="s">
         <v>58</v>
@@ -1788,7 +1791,7 @@
         <v>134</v>
       </c>
       <c r="BU1" s="8" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="BV1" s="1" t="s">
         <v>66</v>
@@ -1874,7 +1877,7 @@
         <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1883,7 +1886,7 @@
         <v>0.02</v>
       </c>
       <c r="G2" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1898,10 +1901,10 @@
         <v>110</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="N2" t="s">
         <v>127</v>
@@ -1910,7 +1913,7 @@
         <v>10</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -1922,7 +1925,7 @@
         <v>0.25</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="X2" t="s">
         <v>131</v>
@@ -1970,13 +1973,13 @@
         <v>0.5</v>
       </c>
       <c r="BM2" s="5" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="BN2">
         <v>0</v>
       </c>
       <c r="BO2" s="5" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="BQ2">
         <v>25</v>
@@ -2020,13 +2023,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -2035,7 +2038,7 @@
         <v>0.02</v>
       </c>
       <c r="G3" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2050,10 +2053,10 @@
         <v>110</v>
       </c>
       <c r="L3" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="M3" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="N3" t="s">
         <v>127</v>
@@ -2062,7 +2065,7 @@
         <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="S3">
         <v>5</v>
@@ -2074,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="V3" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="W3">
         <v>1</v>
@@ -2125,13 +2128,13 @@
         <v>0.5</v>
       </c>
       <c r="BM3" s="5" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="BN3">
         <v>0</v>
       </c>
       <c r="BO3" s="5" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="BQ3">
         <v>25</v>
@@ -2265,7 +2268,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="CR20" s="4"/>
     </row>
@@ -2274,7 +2277,7 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="CR21" s="4">
         <v>45383</v>
@@ -2282,7 +2285,7 @@
     </row>
     <row r="22" spans="1:96">
       <c r="D22" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="CR22" s="4">
         <v>45383</v>
@@ -3565,7 +3568,7 @@
         <v>98</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -3600,7 +3603,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -3716,7 +3719,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -3739,7 +3742,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
         <v>127</v>
@@ -3779,7 +3782,7 @@
         <v>102</v>
       </c>
       <c r="F10" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="H10" t="s">
         <v>49</v>
@@ -3871,18 +3874,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -3890,7 +3893,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -3898,29 +3901,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3940,24 +3943,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="C1" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51">
       <c r="A2" s="1" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated calculate_history_indicators.py for indicators configurations
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Code/Trading/MST50_Trading_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B02401-0B67-F743-9292-1EA5CBA3BC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B50F596-C925-B44B-9C63-CA67DD4B9D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19600" yWindow="29300" windowWidth="33720" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="219">
   <si>
     <t>strategy_name</t>
   </si>
@@ -666,6 +666,33 @@
   </si>
   <si>
     <t>default  0 - not in use</t>
+  </si>
+  <si>
+    <t>15, 20, 25</t>
+  </si>
+  <si>
+    <t>75, 200, 500</t>
+  </si>
+  <si>
+    <t>No. of touch</t>
+  </si>
+  <si>
+    <t>3, 4, 5</t>
+  </si>
+  <si>
+    <t>5, 10, 15</t>
+  </si>
+  <si>
+    <t>Rejection Multiplier (ATR)</t>
+  </si>
+  <si>
+    <t>Slack for SR (ATR - divider)</t>
+  </si>
+  <si>
+    <t>0.5, 1.0, 1.5</t>
+  </si>
+  <si>
+    <t>2, 7, 14, 21, 50</t>
   </si>
 </sst>
 </file>
@@ -1541,11 +1568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS386"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CO2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="172" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CR2" sqref="CR2"/>
+      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -3877,15 +3904,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F67585E-4D72-7443-8AD2-BC7E225DC07C}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -3895,8 +3925,17 @@
       <c r="C1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -3904,26 +3943,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>144</v>
       </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>145</v>
       </c>
-      <c r="B4">
-        <v>14</v>
+      <c r="B4" t="s">
+        <v>210</v>
       </c>
       <c r="C4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -3931,12 +3970,29 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>148</v>
       </c>
       <c r="B6" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>